<commit_message>
cache available labs query; added more panels; improved sticky headers
</commit_message>
<xml_diff>
--- a/storage/lab_lookup.xlsx
+++ b/storage/lab_lookup.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stringali/www/cprs-labs/storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86728D58-3708-6549-8FFD-8EDC75798139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB5B9FB-88C2-FB43-B8B8-A9E729D34B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" xr2:uid="{EC4C72D0-1B9F-7D49-8CE6-24171288DA42}"/>
   </bookViews>
   <sheets>
     <sheet name="labs" sheetId="1" r:id="rId1"/>
+    <sheet name="panesl" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="289">
   <si>
     <t>WBC</t>
   </si>
@@ -672,6 +673,237 @@
   </si>
   <si>
     <t>C. Diff Tox B PCR</t>
+  </si>
+  <si>
+    <t>CBC</t>
+  </si>
+  <si>
+    <t>Morphology</t>
+  </si>
+  <si>
+    <t>Chem</t>
+  </si>
+  <si>
+    <t>LFT</t>
+  </si>
+  <si>
+    <t>ABG</t>
+  </si>
+  <si>
+    <t>Coag</t>
+  </si>
+  <si>
+    <t>Cardiac</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>Infectious</t>
+  </si>
+  <si>
+    <t>Body Fluids</t>
+  </si>
+  <si>
+    <t>Urine</t>
+  </si>
+  <si>
+    <t>UDS</t>
+  </si>
+  <si>
+    <t>AMPHETAMINES SCREEN,urine</t>
+  </si>
+  <si>
+    <t>BARBITURATES SCREEN,urine</t>
+  </si>
+  <si>
+    <t>BENZODIAZEPINES SCREEN,urine</t>
+  </si>
+  <si>
+    <t>CANNABINOIDS SCREEN,urine</t>
+  </si>
+  <si>
+    <t>COCAINE SCREEN,urine</t>
+  </si>
+  <si>
+    <t>METHADONE SCREEN,urine</t>
+  </si>
+  <si>
+    <t>OPIATES SCREEN,urine</t>
+  </si>
+  <si>
+    <t>OXYCODONE SCREEN,urine</t>
+  </si>
+  <si>
+    <t>PHENCYCLIDINE SCREEN,urine</t>
+  </si>
+  <si>
+    <t>Amphetamines</t>
+  </si>
+  <si>
+    <t>Barbiturates</t>
+  </si>
+  <si>
+    <t>Benzodiazepines</t>
+  </si>
+  <si>
+    <t>Cannabinoids</t>
+  </si>
+  <si>
+    <t>Cocaine</t>
+  </si>
+  <si>
+    <t>Methadone</t>
+  </si>
+  <si>
+    <t>Opiates</t>
+  </si>
+  <si>
+    <t>Oxycodone</t>
+  </si>
+  <si>
+    <t>Phencyclidine</t>
+  </si>
+  <si>
+    <t>Creatinine, Urine</t>
+  </si>
+  <si>
+    <t>C-REACTIVE PROTEIN,BLOOD</t>
+  </si>
+  <si>
+    <t>PROCALCITONIN,BLOOD</t>
+  </si>
+  <si>
+    <t>VANCOMYCIN-TROUGH,BLOOD</t>
+  </si>
+  <si>
+    <t>VANCOMYCIN-RANDOM,BLOOD</t>
+  </si>
+  <si>
+    <t>ESR,BLOOD</t>
+  </si>
+  <si>
+    <t>LACTIC ACID,BLOOD</t>
+  </si>
+  <si>
+    <t>AMMONIA,BLOOD</t>
+  </si>
+  <si>
+    <t>PROLACTIN,BLOOD</t>
+  </si>
+  <si>
+    <t>TSH,BLOOD</t>
+  </si>
+  <si>
+    <t>ETHANOL,Urine</t>
+  </si>
+  <si>
+    <t>EtOH</t>
+  </si>
+  <si>
+    <t>CRP</t>
+  </si>
+  <si>
+    <t>Procalcitonin</t>
+  </si>
+  <si>
+    <t>Vanco, Random</t>
+  </si>
+  <si>
+    <t>Vanco, Trough</t>
+  </si>
+  <si>
+    <t>ESR</t>
+  </si>
+  <si>
+    <t>Lactic Acid</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Prolactin</t>
+  </si>
+  <si>
+    <t>TSH</t>
+  </si>
+  <si>
+    <t>TARGET CELLS</t>
+  </si>
+  <si>
+    <t>Target Cells</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Vitamins</t>
+  </si>
+  <si>
+    <t>Autoimmune</t>
+  </si>
+  <si>
+    <t>FOLATE,Blood</t>
+  </si>
+  <si>
+    <t>VITAMIN B12,Blood</t>
+  </si>
+  <si>
+    <t>Folate</t>
+  </si>
+  <si>
+    <t>Vit B12</t>
+  </si>
+  <si>
+    <t>COVID-19 (CEPHEID)</t>
+  </si>
+  <si>
+    <t>COVID-19 ANTIGEN (BINAX)</t>
+  </si>
+  <si>
+    <t>COVID-19 PCR (FLUVID)</t>
+  </si>
+  <si>
+    <t>FLU B PCR (FLUVID)</t>
+  </si>
+  <si>
+    <t>COVID-19 Antigen</t>
+  </si>
+  <si>
+    <t>COVID-19 PCR</t>
+  </si>
+  <si>
+    <t>FLU A PCR</t>
+  </si>
+  <si>
+    <t>FLU B PCR</t>
+  </si>
+  <si>
+    <t>RSV PCR</t>
+  </si>
+  <si>
+    <t>Misc Chemistry</t>
+  </si>
+  <si>
+    <t>RSV PCR (FLUVID)</t>
+  </si>
+  <si>
+    <t>FLU A PCR (FLUVID)</t>
+  </si>
+  <si>
+    <t>Glucose, POC</t>
+  </si>
+  <si>
+    <t>GLUCOSE,POC</t>
+  </si>
+  <si>
+    <t>LIPASE,BLOOD</t>
+  </si>
+  <si>
+    <t>Lipase</t>
+  </si>
+  <si>
+    <t>CREATININE,Urine</t>
   </si>
 </sst>
 </file>
@@ -1023,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD366CC-41DC-0B48-90D3-657EFDB6DEEB}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="E113" sqref="E112:E113"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="E144" sqref="E2:E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1083,7 +1315,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">"['panel_id' =&gt; '"&amp;A3&amp;"', 'name' =&gt; '"&amp;B3&amp;"', 'label' =&gt; '"&amp;C3&amp;"', 'sort_id' =&gt; '"&amp;D3&amp;"'],"</f>
+        <f t="shared" ref="E3:E68" si="0">"['panel_id' =&gt; '"&amp;A3&amp;"', 'name' =&gt; '"&amp;B3&amp;"', 'label' =&gt; '"&amp;C3&amp;"', 'sort_id' =&gt; '"&amp;D3&amp;"'],"</f>
         <v>['panel_id' =&gt; '1', 'name' =&gt; 'RBC', 'label' =&gt; 'RBC', 'sort_id' =&gt; '2'],</v>
       </c>
     </row>
@@ -1884,17 +2116,17 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>263</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>264</v>
       </c>
       <c r="D48">
         <v>47</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'SCHISTOCYTES', 'label' =&gt; 'Schistocytes', 'sort_id' =&gt; '47'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'TARGET CELLS', 'label' =&gt; 'Target Cells', 'sort_id' =&gt; '47'],</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1902,17 +2134,17 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D49">
         <v>48</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'SPHEROCYTES', 'label' =&gt; 'Spherocytes', 'sort_id' =&gt; '48'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'SCHISTOCYTES', 'label' =&gt; 'Schistocytes', 'sort_id' =&gt; '48'],</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1920,17 +2152,17 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D50">
         <v>49</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'OVALOCYTES', 'label' =&gt; 'Ovalocytes', 'sort_id' =&gt; '49'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'SPHEROCYTES', 'label' =&gt; 'Spherocytes', 'sort_id' =&gt; '49'],</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1938,17 +2170,17 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D51">
         <v>50</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'STOMATOCYTE', 'label' =&gt; 'Stomatocyte', 'sort_id' =&gt; '50'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'OVALOCYTES', 'label' =&gt; 'Ovalocytes', 'sort_id' =&gt; '50'],</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1956,17 +2188,17 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D52">
         <v>51</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'BURR CELLS', 'label' =&gt; 'Burr cells', 'sort_id' =&gt; '51'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'STOMATOCYTE', 'label' =&gt; 'Stomatocyte', 'sort_id' =&gt; '51'],</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1974,17 +2206,17 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D53">
         <v>52</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'ACANTHOCYTES', 'label' =&gt; 'Acanthocytes', 'sort_id' =&gt; '52'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'BURR CELLS', 'label' =&gt; 'Burr cells', 'sort_id' =&gt; '52'],</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1992,35 +2224,35 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D54">
         <v>53</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'TEARDROP CELLS', 'label' =&gt; 'Teardrop cells', 'sort_id' =&gt; '53'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'ACANTHOCYTES', 'label' =&gt; 'Acanthocytes', 'sort_id' =&gt; '53'],</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D55">
         <v>54</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'GLUCOSE,Blood', 'label' =&gt; 'Glucose', 'sort_id' =&gt; '54'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'TEARDROP CELLS', 'label' =&gt; 'Teardrop cells', 'sort_id' =&gt; '54'],</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2028,17 +2260,17 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D56">
         <v>55</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'SODIUM,Blood', 'label' =&gt; 'Na', 'sort_id' =&gt; '55'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'GLUCOSE,Blood', 'label' =&gt; 'Glucose', 'sort_id' =&gt; '55'],</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2046,17 +2278,17 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>285</v>
       </c>
       <c r="C57" t="s">
-        <v>155</v>
+        <v>284</v>
       </c>
       <c r="D57">
         <v>56</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'POTASSIUM,Blood', 'label' =&gt; 'K', 'sort_id' =&gt; '56'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'GLUCOSE,POC', 'label' =&gt; 'Glucose, POC', 'sort_id' =&gt; '56'],</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2064,17 +2296,17 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D58">
         <v>57</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CHLORIDE,Blood', 'label' =&gt; 'Cl', 'sort_id' =&gt; '57'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'SODIUM,Blood', 'label' =&gt; 'Na', 'sort_id' =&gt; '57'],</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2082,17 +2314,17 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="D59">
         <v>58</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CARBON DIOXIDE,Blood', 'label' =&gt; 'HCO3', 'sort_id' =&gt; '58'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'POTASSIUM,Blood', 'label' =&gt; 'K', 'sort_id' =&gt; '58'],</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2100,17 +2332,17 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D60">
         <v>59</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'UREA NITROGEN,Blood', 'label' =&gt; 'BUN', 'sort_id' =&gt; '59'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CHLORIDE,Blood', 'label' =&gt; 'Cl', 'sort_id' =&gt; '59'],</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2118,17 +2350,17 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>158</v>
+        <v>78</v>
       </c>
       <c r="D61">
         <v>60</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CREATININE,blood', 'label' =&gt; 'Cr', 'sort_id' =&gt; '60'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CARBON DIOXIDE,Blood', 'label' =&gt; 'HCO3', 'sort_id' =&gt; '60'],</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2136,17 +2368,17 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D62">
         <v>61</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CALCIUM,Blood', 'label' =&gt; 'Calcium', 'sort_id' =&gt; '61'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'UREA NITROGEN,Blood', 'label' =&gt; 'BUN', 'sort_id' =&gt; '61'],</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2154,17 +2386,17 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D63">
         <v>62</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'ANION GAP,blood', 'label' =&gt; 'Anion Gap', 'sort_id' =&gt; '62'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CREATININE,blood', 'label' =&gt; 'Cr', 'sort_id' =&gt; '62'],</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2172,53 +2404,53 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D64">
         <v>63</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'EGFR CKD,blood', 'label' =&gt; 'EGFR', 'sort_id' =&gt; '63'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CALCIUM,Blood', 'label' =&gt; 'Calcium', 'sort_id' =&gt; '63'],</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D65">
         <v>64</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'PROTEIN,TOTAL,Blood', 'label' =&gt; 'Protein', 'sort_id' =&gt; '64'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'ANION GAP,blood', 'label' =&gt; 'Anion Gap', 'sort_id' =&gt; '64'],</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D66">
         <v>65</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALBUMIN ,Blood', 'label' =&gt; 'Albumin', 'sort_id' =&gt; '65'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'EGFR CKD,blood', 'label' =&gt; 'EGFR', 'sort_id' =&gt; '65'],</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2226,17 +2458,17 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D67">
         <v>66</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E113" si="1">"['panel_id' =&gt; '"&amp;A67&amp;"', 'name' =&gt; '"&amp;B67&amp;"', 'label' =&gt; '"&amp;C67&amp;"', 'sort_id' =&gt; '"&amp;D67&amp;"'],"</f>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'BILIRUBIN,TOTAL,Blood', 'label' =&gt; 'T-Bili', 'sort_id' =&gt; '66'],</v>
+        <f t="shared" si="0"/>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'PROTEIN,TOTAL,Blood', 'label' =&gt; 'Protein', 'sort_id' =&gt; '66'],</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -2244,17 +2476,17 @@
         <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C68" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D68">
         <v>67</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'BILIRUBIN,DIRECT,blood', 'label' =&gt; 'D-Bili', 'sort_id' =&gt; '67'],</v>
+        <f t="shared" si="0"/>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALBUMIN ,Blood', 'label' =&gt; 'Albumin', 'sort_id' =&gt; '67'],</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2262,17 +2494,17 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C69" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D69">
         <v>68</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALKP,Blood', 'label' =&gt; 'ALKP', 'sort_id' =&gt; '68'],</v>
+        <f t="shared" ref="E69:E135" si="1">"['panel_id' =&gt; '"&amp;A69&amp;"', 'name' =&gt; '"&amp;B69&amp;"', 'label' =&gt; '"&amp;C69&amp;"', 'sort_id' =&gt; '"&amp;D69&amp;"'],"</f>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'BILIRUBIN,TOTAL,Blood', 'label' =&gt; 'T-Bili', 'sort_id' =&gt; '68'],</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -2280,17 +2512,17 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C70" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D70">
         <v>69</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALT,Blood', 'label' =&gt; 'ALT', 'sort_id' =&gt; '69'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'BILIRUBIN,DIRECT,blood', 'label' =&gt; 'D-Bili', 'sort_id' =&gt; '69'],</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -2298,17 +2530,17 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C71" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D71">
         <v>70</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'AST,Blood', 'label' =&gt; 'AST', 'sort_id' =&gt; '70'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALKP,Blood', 'label' =&gt; 'ALKP', 'sort_id' =&gt; '70'],</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -2316,17 +2548,17 @@
         <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D72">
         <v>71</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'MAGNESIUM,Blood', 'label' =&gt; 'Mg', 'sort_id' =&gt; '71'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALT,Blood', 'label' =&gt; 'ALT', 'sort_id' =&gt; '71'],</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -2334,53 +2566,53 @@
         <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D73">
         <v>72</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'PHOSPHORUS,Blood', 'label' =&gt; 'PO4', 'sort_id' =&gt; '72'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'AST,Blood', 'label' =&gt; 'AST', 'sort_id' =&gt; '72'],</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C74" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="D74">
         <v>73</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'SODIUM,ISTAT', 'label' =&gt; 'Na', 'sort_id' =&gt; '73'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'MAGNESIUM,Blood', 'label' =&gt; 'Mg', 'sort_id' =&gt; '73'],</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="D75">
         <v>74</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'POTASSIUM,ISTAT', 'label' =&gt; 'K', 'sort_id' =&gt; '74'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'PHOSPHORUS,Blood', 'label' =&gt; 'PO4', 'sort_id' =&gt; '74'],</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -2388,17 +2620,17 @@
         <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C76" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="D76">
         <v>75</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PH @ 37C', 'label' =&gt; 'pH', 'sort_id' =&gt; '75'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'SODIUM,ISTAT', 'label' =&gt; 'Na', 'sort_id' =&gt; '75'],</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2406,17 +2638,17 @@
         <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C77" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="D77">
         <v>76</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PCO2 @ 37C', 'label' =&gt; 'PCO2', 'sort_id' =&gt; '76'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'POTASSIUM,ISTAT', 'label' =&gt; 'K', 'sort_id' =&gt; '76'],</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2424,17 +2656,17 @@
         <v>5</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C78" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="D78">
         <v>77</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'TCO2', 'label' =&gt; 'TCO2', 'sort_id' =&gt; '77'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PH @ 37C', 'label' =&gt; 'pH', 'sort_id' =&gt; '77'],</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2442,17 +2674,17 @@
         <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D79">
         <v>78</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PO2 @ 37C', 'label' =&gt; 'PO2', 'sort_id' =&gt; '78'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PCO2 @ 37C', 'label' =&gt; 'PCO2', 'sort_id' =&gt; '78'],</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2460,17 +2692,17 @@
         <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C80" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D80">
         <v>79</v>
       </c>
       <c r="E80" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'HCO3', 'label' =&gt; 'HCO3', 'sort_id' =&gt; '79'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'TCO2', 'label' =&gt; 'TCO2', 'sort_id' =&gt; '79'],</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2478,17 +2710,17 @@
         <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D81">
         <v>80</v>
       </c>
       <c r="E81" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'BASE EXCESS (BE)', 'label' =&gt; 'Base Excess', 'sort_id' =&gt; '80'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PO2 @ 37C', 'label' =&gt; 'PO2', 'sort_id' =&gt; '80'],</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2496,17 +2728,17 @@
         <v>5</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C82" t="s">
-        <v>175</v>
+        <v>78</v>
       </c>
       <c r="D82">
         <v>81</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'O2 SAT%', 'label' =&gt; 'SpO2', 'sort_id' =&gt; '81'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'HCO3', 'label' =&gt; 'HCO3', 'sort_id' =&gt; '81'],</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2514,53 +2746,53 @@
         <v>5</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C83" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="D83">
         <v>82</v>
       </c>
       <c r="E83" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'FIO2', 'label' =&gt; 'FIO2', 'sort_id' =&gt; '82'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'BASE EXCESS (BE)', 'label' =&gt; 'Base Excess', 'sort_id' =&gt; '82'],</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C84" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D84">
         <v>83</v>
       </c>
       <c r="E84" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '6', 'name' =&gt; 'ANTI-Xa(UFH),BLOOD', 'label' =&gt; 'Anit-Xa (UFH)', 'sort_id' =&gt; '83'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'O2 SAT%', 'label' =&gt; 'SpO2', 'sort_id' =&gt; '83'],</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C85" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
       <c r="D85">
         <v>84</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '6', 'name' =&gt; 'PROTHROMBIN TIME,blood', 'label' =&gt; 'PT', 'sort_id' =&gt; '84'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'FIO2', 'label' =&gt; 'FIO2', 'sort_id' =&gt; '84'],</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2568,17 +2800,17 @@
         <v>6</v>
       </c>
       <c r="B86" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C86" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D86">
         <v>85</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '6', 'name' =&gt; 'INR,blood', 'label' =&gt; 'INR', 'sort_id' =&gt; '85'],</v>
+        <v>['panel_id' =&gt; '6', 'name' =&gt; 'ANTI-Xa(UFH),BLOOD', 'label' =&gt; 'Anit-Xa (UFH)', 'sort_id' =&gt; '85'],</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2586,53 +2818,53 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C87" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D87">
         <v>86</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '6', 'name' =&gt; 'APTT', 'label' =&gt; 'aPTT', 'sort_id' =&gt; '86'],</v>
+        <v>['panel_id' =&gt; '6', 'name' =&gt; 'PROTHROMBIN TIME,blood', 'label' =&gt; 'PT', 'sort_id' =&gt; '86'],</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C88" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D88">
         <v>87</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'BNP,BLOOD', 'label' =&gt; 'BNP', 'sort_id' =&gt; '87'],</v>
+        <v>['panel_id' =&gt; '6', 'name' =&gt; 'INR,blood', 'label' =&gt; 'INR', 'sort_id' =&gt; '87'],</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C89" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D89">
         <v>88</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CK,Blood', 'label' =&gt; 'CK', 'sort_id' =&gt; '88'],</v>
+        <v>['panel_id' =&gt; '6', 'name' =&gt; 'APTT', 'label' =&gt; 'aPTT', 'sort_id' =&gt; '88'],</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2640,17 +2872,17 @@
         <v>7</v>
       </c>
       <c r="B90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C90" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D90">
         <v>89</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CKMB,blood', 'label' =&gt; 'CKMB', 'sort_id' =&gt; '89'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'BNP,BLOOD', 'label' =&gt; 'BNP', 'sort_id' =&gt; '89'],</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -2658,17 +2890,17 @@
         <v>7</v>
       </c>
       <c r="B91" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C91" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D91">
         <v>90</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CKMB INDEX,blood', 'label' =&gt; 'CKMB Index', 'sort_id' =&gt; '90'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CK,Blood', 'label' =&gt; 'CK', 'sort_id' =&gt; '90'],</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2676,17 +2908,17 @@
         <v>7</v>
       </c>
       <c r="B92" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C92" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D92">
         <v>91</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'MYOGLOBIN,Blood', 'label' =&gt; 'Myoglobin', 'sort_id' =&gt; '91'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CKMB,blood', 'label' =&gt; 'CKMB', 'sort_id' =&gt; '91'],</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2694,53 +2926,53 @@
         <v>7</v>
       </c>
       <c r="B93" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C93" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D93">
         <v>92</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'TROPONIN-I,BLOOD', 'label' =&gt; 'Troponin-I', 'sort_id' =&gt; '92'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CKMB INDEX,blood', 'label' =&gt; 'CKMB Index', 'sort_id' =&gt; '92'],</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B94" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C94" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D94">
         <v>93</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE GLUCOSE', 'label' =&gt; 'Urine Glucose', 'sort_id' =&gt; '93'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'MYOGLOBIN,Blood', 'label' =&gt; 'Myoglobin', 'sort_id' =&gt; '93'],</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B95" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C95" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D95">
         <v>94</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE PROTEIN', 'label' =&gt; 'Urine Protein', 'sort_id' =&gt; '94'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'TROPONIN-I,BLOOD', 'label' =&gt; 'Troponin-I', 'sort_id' =&gt; '94'],</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2748,17 +2980,17 @@
         <v>8</v>
       </c>
       <c r="B96" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D96">
         <v>95</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BILIRUBIN', 'label' =&gt; 'Urine Bilirubin', 'sort_id' =&gt; '95'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE GLUCOSE', 'label' =&gt; 'Urine Glucose', 'sort_id' =&gt; '95'],</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -2766,17 +2998,17 @@
         <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C97" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D97">
         <v>96</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE UROBILINOGEN', 'label' =&gt; 'Urine Urobilinogen', 'sort_id' =&gt; '96'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE PROTEIN', 'label' =&gt; 'Urine Protein', 'sort_id' =&gt; '96'],</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -2784,17 +3016,17 @@
         <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C98" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D98">
         <v>97</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE PH', 'label' =&gt; 'Urine pH', 'sort_id' =&gt; '97'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BILIRUBIN', 'label' =&gt; 'Urine Bilirubin', 'sort_id' =&gt; '97'],</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -2802,17 +3034,17 @@
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C99" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D99">
         <v>98</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BLOOD', 'label' =&gt; 'Urine Blood', 'sort_id' =&gt; '98'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE UROBILINOGEN', 'label' =&gt; 'Urine Urobilinogen', 'sort_id' =&gt; '98'],</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -2820,17 +3052,17 @@
         <v>8</v>
       </c>
       <c r="B100" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C100" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D100">
         <v>99</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE KETONES', 'label' =&gt; 'Urine Ketones', 'sort_id' =&gt; '99'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE PH', 'label' =&gt; 'Urine pH', 'sort_id' =&gt; '99'],</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -2838,17 +3070,17 @@
         <v>8</v>
       </c>
       <c r="B101" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C101" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D101">
         <v>100</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE NITRITE', 'label' =&gt; 'Urine Nitrite', 'sort_id' =&gt; '100'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BLOOD', 'label' =&gt; 'Urine Blood', 'sort_id' =&gt; '100'],</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -2856,17 +3088,17 @@
         <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C102" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D102">
         <v>101</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE LEUKOCYTE ESTERASE', 'label' =&gt; 'Urine Leukocyte Esterase', 'sort_id' =&gt; '101'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE KETONES', 'label' =&gt; 'Urine Ketones', 'sort_id' =&gt; '101'],</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -2874,17 +3106,17 @@
         <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D103">
         <v>102</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE CLARITY', 'label' =&gt; 'Urine Clarity', 'sort_id' =&gt; '102'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE NITRITE', 'label' =&gt; 'Urine Nitrite', 'sort_id' =&gt; '102'],</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -2892,17 +3124,17 @@
         <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C104" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D104">
         <v>103</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE SPECIFIC GRAVITY', 'label' =&gt; 'Urine Sp Gravity', 'sort_id' =&gt; '103'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE LEUKOCYTE ESTERASE', 'label' =&gt; 'Urine Leukocyte Esterase', 'sort_id' =&gt; '103'],</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -2910,17 +3142,17 @@
         <v>8</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C105" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D105">
         <v>104</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE COLOR', 'label' =&gt; 'Urine Color', 'sort_id' =&gt; '104'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE CLARITY', 'label' =&gt; 'Urine Clarity', 'sort_id' =&gt; '104'],</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -2928,17 +3160,17 @@
         <v>8</v>
       </c>
       <c r="B106" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C106" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D106">
         <v>105</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'RBC/HPF', 'label' =&gt; 'RBC/Hpf', 'sort_id' =&gt; '105'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE SPECIFIC GRAVITY', 'label' =&gt; 'Urine Sp Gravity', 'sort_id' =&gt; '105'],</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -2946,17 +3178,17 @@
         <v>8</v>
       </c>
       <c r="B107" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C107" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D107">
         <v>106</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'WBC/HPF', 'label' =&gt; 'WBC/Hpf', 'sort_id' =&gt; '106'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE COLOR', 'label' =&gt; 'Urine Color', 'sort_id' =&gt; '106'],</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -2964,17 +3196,17 @@
         <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C108" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D108">
         <v>107</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BACTERIA', 'label' =&gt; 'Urine Bacteria', 'sort_id' =&gt; '107'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'RBC/HPF', 'label' =&gt; 'RBC/Hpf', 'sort_id' =&gt; '107'],</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -2982,17 +3214,17 @@
         <v>8</v>
       </c>
       <c r="B109" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C109" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D109">
         <v>108</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'SQUAMOUS EPITHELIAL', 'label' =&gt; 'Squamous Epithelial', 'sort_id' =&gt; '108'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'WBC/HPF', 'label' =&gt; 'WBC/Hpf', 'sort_id' =&gt; '108'],</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -3000,17 +3232,17 @@
         <v>8</v>
       </c>
       <c r="B110" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C110" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D110">
         <v>109</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'HYALINE CAST', 'label' =&gt; 'Hyaline Cast', 'sort_id' =&gt; '109'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BACTERIA', 'label' =&gt; 'Urine Bacteria', 'sort_id' =&gt; '109'],</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -3018,53 +3250,881 @@
         <v>8</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C111" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D111">
         <v>110</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'CALCIUM OXALATE', 'label' =&gt; 'Calcium Oxalate', 'sort_id' =&gt; '110'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'SQUAMOUS EPITHELIAL', 'label' =&gt; 'Squamous Epithelial', 'sort_id' =&gt; '110'],</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B112" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C112" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D112">
         <v>111</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '9', 'name' =&gt; 'C. DIFF TOX B GENE PCR,stool', 'label' =&gt; 'C. Diff Tox B PCR', 'sort_id' =&gt; '111'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'HYALINE CAST', 'label' =&gt; 'Hyaline Cast', 'sort_id' =&gt; '111'],</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B113" t="s">
-        <v>208</v>
+        <v>109</v>
       </c>
       <c r="C113" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D113">
         <v>112</v>
       </c>
       <c r="E113" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '9', 'name' =&gt; 'VZ DNA', 'label' =&gt; 'VZV DNA PCR', 'sort_id' =&gt; '112'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'CALCIUM OXALATE', 'label' =&gt; 'Calcium Oxalate', 'sort_id' =&gt; '112'],</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>9</v>
+      </c>
+      <c r="B114" t="s">
+        <v>210</v>
+      </c>
+      <c r="C114" t="s">
+        <v>211</v>
+      </c>
+      <c r="D114">
+        <v>113</v>
+      </c>
+      <c r="E114" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'C. DIFF TOX B GENE PCR,stool', 'label' =&gt; 'C. Diff Tox B PCR', 'sort_id' =&gt; '113'],</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>9</v>
+      </c>
+      <c r="B115" t="s">
+        <v>208</v>
+      </c>
+      <c r="C115" t="s">
+        <v>209</v>
+      </c>
+      <c r="D115">
+        <v>114</v>
+      </c>
+      <c r="E115" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'VZ DNA', 'label' =&gt; 'VZV DNA PCR', 'sort_id' =&gt; '114'],</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>12</v>
+      </c>
+      <c r="B116" t="s">
+        <v>252</v>
+      </c>
+      <c r="C116" t="s">
+        <v>253</v>
+      </c>
+      <c r="D116">
+        <v>115</v>
+      </c>
+      <c r="E116" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'ETHANOL,Urine', 'label' =&gt; 'EtOH', 'sort_id' =&gt; '115'],</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>12</v>
+      </c>
+      <c r="B117" t="s">
+        <v>224</v>
+      </c>
+      <c r="C117" t="s">
+        <v>233</v>
+      </c>
+      <c r="D117">
+        <v>116</v>
+      </c>
+      <c r="E117" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'AMPHETAMINES SCREEN,urine', 'label' =&gt; 'Amphetamines', 'sort_id' =&gt; '116'],</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>12</v>
+      </c>
+      <c r="B118" t="s">
+        <v>225</v>
+      </c>
+      <c r="C118" t="s">
+        <v>234</v>
+      </c>
+      <c r="D118">
+        <v>117</v>
+      </c>
+      <c r="E118" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'BARBITURATES SCREEN,urine', 'label' =&gt; 'Barbiturates', 'sort_id' =&gt; '117'],</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>12</v>
+      </c>
+      <c r="B119" t="s">
+        <v>226</v>
+      </c>
+      <c r="C119" t="s">
+        <v>235</v>
+      </c>
+      <c r="D119">
+        <v>118</v>
+      </c>
+      <c r="E119" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'BENZODIAZEPINES SCREEN,urine', 'label' =&gt; 'Benzodiazepines', 'sort_id' =&gt; '118'],</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>12</v>
+      </c>
+      <c r="B120" t="s">
+        <v>227</v>
+      </c>
+      <c r="C120" t="s">
+        <v>236</v>
+      </c>
+      <c r="D120">
+        <v>119</v>
+      </c>
+      <c r="E120" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'CANNABINOIDS SCREEN,urine', 'label' =&gt; 'Cannabinoids', 'sort_id' =&gt; '119'],</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>12</v>
+      </c>
+      <c r="B121" t="s">
+        <v>228</v>
+      </c>
+      <c r="C121" t="s">
+        <v>237</v>
+      </c>
+      <c r="D121">
+        <v>120</v>
+      </c>
+      <c r="E121" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'COCAINE SCREEN,urine', 'label' =&gt; 'Cocaine', 'sort_id' =&gt; '120'],</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>12</v>
+      </c>
+      <c r="B122" t="s">
+        <v>229</v>
+      </c>
+      <c r="C122" t="s">
+        <v>238</v>
+      </c>
+      <c r="D122">
+        <v>121</v>
+      </c>
+      <c r="E122" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'METHADONE SCREEN,urine', 'label' =&gt; 'Methadone', 'sort_id' =&gt; '121'],</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>12</v>
+      </c>
+      <c r="B123" t="s">
+        <v>230</v>
+      </c>
+      <c r="C123" t="s">
+        <v>239</v>
+      </c>
+      <c r="D123">
+        <v>122</v>
+      </c>
+      <c r="E123" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'OPIATES SCREEN,urine', 'label' =&gt; 'Opiates', 'sort_id' =&gt; '122'],</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>12</v>
+      </c>
+      <c r="B124" t="s">
+        <v>231</v>
+      </c>
+      <c r="C124" t="s">
+        <v>240</v>
+      </c>
+      <c r="D124">
+        <v>123</v>
+      </c>
+      <c r="E124" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'OXYCODONE SCREEN,urine', 'label' =&gt; 'Oxycodone', 'sort_id' =&gt; '123'],</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>12</v>
+      </c>
+      <c r="B125" t="s">
+        <v>232</v>
+      </c>
+      <c r="C125" t="s">
+        <v>241</v>
+      </c>
+      <c r="D125">
+        <v>124</v>
+      </c>
+      <c r="E125" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'PHENCYCLIDINE SCREEN,urine', 'label' =&gt; 'Phencyclidine', 'sort_id' =&gt; '124'],</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>11</v>
+      </c>
+      <c r="B126" t="s">
+        <v>288</v>
+      </c>
+      <c r="C126" t="s">
+        <v>242</v>
+      </c>
+      <c r="D126">
+        <v>125</v>
+      </c>
+      <c r="E126" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '11', 'name' =&gt; 'CREATININE,Urine', 'label' =&gt; 'Creatinine, Urine', 'sort_id' =&gt; '125'],</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>5</v>
+      </c>
+      <c r="B127" t="s">
+        <v>251</v>
+      </c>
+      <c r="C127" t="s">
+        <v>262</v>
+      </c>
+      <c r="D127">
+        <v>126</v>
+      </c>
+      <c r="E127" t="str">
+        <f>"['panel_id' =&gt; '"&amp;A127&amp;"', 'name' =&gt; '"&amp;B127&amp;"', 'label' =&gt; '"&amp;C127&amp;"', 'sort_id' =&gt; '"&amp;D127&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'TSH,BLOOD', 'label' =&gt; 'TSH', 'sort_id' =&gt; '126'],</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>5</v>
+      </c>
+      <c r="B128" t="s">
+        <v>249</v>
+      </c>
+      <c r="C128" t="s">
+        <v>260</v>
+      </c>
+      <c r="D128">
+        <v>127</v>
+      </c>
+      <c r="E128" t="str">
+        <f>"['panel_id' =&gt; '"&amp;A128&amp;"', 'name' =&gt; '"&amp;B128&amp;"', 'label' =&gt; '"&amp;C128&amp;"', 'sort_id' =&gt; '"&amp;D128&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'AMMONIA,BLOOD', 'label' =&gt; 'Ammonia', 'sort_id' =&gt; '127'],</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>5</v>
+      </c>
+      <c r="B129" t="s">
+        <v>248</v>
+      </c>
+      <c r="C129" t="s">
+        <v>259</v>
+      </c>
+      <c r="D129">
+        <v>128</v>
+      </c>
+      <c r="E129" t="str">
+        <f>"['panel_id' =&gt; '"&amp;A129&amp;"', 'name' =&gt; '"&amp;B129&amp;"', 'label' =&gt; '"&amp;C129&amp;"', 'sort_id' =&gt; '"&amp;D129&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'LACTIC ACID,BLOOD', 'label' =&gt; 'Lactic Acid', 'sort_id' =&gt; '128'],</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>5</v>
+      </c>
+      <c r="B130" t="s">
+        <v>286</v>
+      </c>
+      <c r="C130" t="s">
+        <v>287</v>
+      </c>
+      <c r="D130">
+        <v>129</v>
+      </c>
+      <c r="E130" t="str">
+        <f>"['panel_id' =&gt; '"&amp;A130&amp;"', 'name' =&gt; '"&amp;B130&amp;"', 'label' =&gt; '"&amp;C130&amp;"', 'sort_id' =&gt; '"&amp;D130&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'LIPASE,BLOOD', 'label' =&gt; 'Lipase', 'sort_id' =&gt; '129'],</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>5</v>
+      </c>
+      <c r="B131" t="s">
+        <v>247</v>
+      </c>
+      <c r="C131" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131">
+        <v>130</v>
+      </c>
+      <c r="E131" t="str">
+        <f>"['panel_id' =&gt; '"&amp;A131&amp;"', 'name' =&gt; '"&amp;B131&amp;"', 'label' =&gt; '"&amp;C131&amp;"', 'sort_id' =&gt; '"&amp;D131&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'ESR,BLOOD', 'label' =&gt; 'ESR', 'sort_id' =&gt; '130'],</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>5</v>
+      </c>
+      <c r="B132" t="s">
+        <v>243</v>
+      </c>
+      <c r="C132" t="s">
+        <v>254</v>
+      </c>
+      <c r="D132">
+        <v>131</v>
+      </c>
+      <c r="E132" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'C-REACTIVE PROTEIN,BLOOD', 'label' =&gt; 'CRP', 'sort_id' =&gt; '131'],</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>5</v>
+      </c>
+      <c r="B133" t="s">
+        <v>244</v>
+      </c>
+      <c r="C133" t="s">
+        <v>255</v>
+      </c>
+      <c r="D133">
+        <v>132</v>
+      </c>
+      <c r="E133" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PROCALCITONIN,BLOOD', 'label' =&gt; 'Procalcitonin', 'sort_id' =&gt; '132'],</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>5</v>
+      </c>
+      <c r="B134" t="s">
+        <v>245</v>
+      </c>
+      <c r="C134" t="s">
+        <v>257</v>
+      </c>
+      <c r="D134">
+        <v>133</v>
+      </c>
+      <c r="E134" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'VANCOMYCIN-TROUGH,BLOOD', 'label' =&gt; 'Vanco, Trough', 'sort_id' =&gt; '133'],</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>5</v>
+      </c>
+      <c r="B135" t="s">
+        <v>246</v>
+      </c>
+      <c r="C135" t="s">
+        <v>256</v>
+      </c>
+      <c r="D135">
+        <v>134</v>
+      </c>
+      <c r="E135" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'VANCOMYCIN-RANDOM,BLOOD', 'label' =&gt; 'Vanco, Random', 'sort_id' =&gt; '134'],</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>5</v>
+      </c>
+      <c r="B136" t="s">
+        <v>250</v>
+      </c>
+      <c r="C136" t="s">
+        <v>261</v>
+      </c>
+      <c r="D136">
+        <v>135</v>
+      </c>
+      <c r="E136" t="str">
+        <f t="shared" ref="E136:E144" si="2">"['panel_id' =&gt; '"&amp;A136&amp;"', 'name' =&gt; '"&amp;B136&amp;"', 'label' =&gt; '"&amp;C136&amp;"', 'sort_id' =&gt; '"&amp;D136&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PROLACTIN,BLOOD', 'label' =&gt; 'Prolactin', 'sort_id' =&gt; '135'],</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>15</v>
+      </c>
+      <c r="B137" t="s">
+        <v>268</v>
+      </c>
+      <c r="C137" t="s">
+        <v>270</v>
+      </c>
+      <c r="D137">
+        <v>136</v>
+      </c>
+      <c r="E137" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '15', 'name' =&gt; 'FOLATE,Blood', 'label' =&gt; 'Folate', 'sort_id' =&gt; '136'],</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>15</v>
+      </c>
+      <c r="B138" t="s">
+        <v>269</v>
+      </c>
+      <c r="C138" t="s">
+        <v>271</v>
+      </c>
+      <c r="D138">
+        <v>137</v>
+      </c>
+      <c r="E138" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '15', 'name' =&gt; 'VITAMIN B12,Blood', 'label' =&gt; 'Vit B12', 'sort_id' =&gt; '137'],</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>9</v>
+      </c>
+      <c r="B139" t="s">
+        <v>272</v>
+      </c>
+      <c r="C139" t="s">
+        <v>277</v>
+      </c>
+      <c r="D139">
+        <v>138</v>
+      </c>
+      <c r="E139" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'COVID-19 (CEPHEID)', 'label' =&gt; 'COVID-19 PCR', 'sort_id' =&gt; '138'],</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>9</v>
+      </c>
+      <c r="B140" t="s">
+        <v>273</v>
+      </c>
+      <c r="C140" t="s">
+        <v>276</v>
+      </c>
+      <c r="D140">
+        <v>139</v>
+      </c>
+      <c r="E140" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'COVID-19 ANTIGEN (BINAX)', 'label' =&gt; 'COVID-19 Antigen', 'sort_id' =&gt; '139'],</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>9</v>
+      </c>
+      <c r="B141" t="s">
+        <v>274</v>
+      </c>
+      <c r="C141" t="s">
+        <v>277</v>
+      </c>
+      <c r="D141">
+        <v>140</v>
+      </c>
+      <c r="E141" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'COVID-19 PCR (FLUVID)', 'label' =&gt; 'COVID-19 PCR', 'sort_id' =&gt; '140'],</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>9</v>
+      </c>
+      <c r="B142" t="s">
+        <v>283</v>
+      </c>
+      <c r="C142" t="s">
+        <v>278</v>
+      </c>
+      <c r="D142">
+        <v>141</v>
+      </c>
+      <c r="E142" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'FLU A PCR (FLUVID)', 'label' =&gt; 'FLU A PCR', 'sort_id' =&gt; '141'],</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>9</v>
+      </c>
+      <c r="B143" t="s">
+        <v>275</v>
+      </c>
+      <c r="C143" t="s">
+        <v>279</v>
+      </c>
+      <c r="D143">
+        <v>142</v>
+      </c>
+      <c r="E143" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'FLU B PCR (FLUVID)', 'label' =&gt; 'FLU B PCR', 'sort_id' =&gt; '142'],</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>9</v>
+      </c>
+      <c r="B144" t="s">
+        <v>282</v>
+      </c>
+      <c r="C144" t="s">
+        <v>280</v>
+      </c>
+      <c r="D144">
+        <v>143</v>
+      </c>
+      <c r="E144" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'RSV PCR (FLUVID)', 'label' =&gt; 'RSV PCR', 'sort_id' =&gt; '143'],</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC0B4A5-5A2B-6C43-ADFA-43D0E3B93788}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"['id' =&gt; "&amp;A2 &amp;", 'label' =&gt; '"&amp;B2 &amp;"', 'sort_id' =&gt; "&amp;C2 &amp;"],"</f>
+        <v>['id' =&gt; 1, 'label' =&gt; 'CBC', 'sort_id' =&gt; 1],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D17" si="0">"['id' =&gt; "&amp;A3 &amp;", 'label' =&gt; '"&amp;B3 &amp;"', 'sort_id' =&gt; "&amp;C3 &amp;"],"</f>
+        <v>['id' =&gt; 2, 'label' =&gt; 'Morphology', 'sort_id' =&gt; 2],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 3, 'label' =&gt; 'Chem', 'sort_id' =&gt; 3],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 4, 'label' =&gt; 'LFT', 'sort_id' =&gt; 4],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 5, 'label' =&gt; 'ABG', 'sort_id' =&gt; 5],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 6, 'label' =&gt; 'Coag', 'sort_id' =&gt; 7],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 7, 'label' =&gt; 'Cardiac', 'sort_id' =&gt; 8],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 8, 'label' =&gt; 'UA', 'sort_id' =&gt; 9],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 9, 'label' =&gt; 'Infectious', 'sort_id' =&gt; 10],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 10, 'label' =&gt; 'Body Fluids', 'sort_id' =&gt; 11],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 11, 'label' =&gt; 'Urine', 'sort_id' =&gt; 12],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 12, 'label' =&gt; 'UDS', 'sort_id' =&gt; 13],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 13, 'label' =&gt; 'Misc Chemistry', 'sort_id' =&gt; 5],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>265</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 14, 'label' =&gt; 'Iron', 'sort_id' =&gt; 14],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 15, 'label' =&gt; 'Vitamins', 'sort_id' =&gt; 15],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>267</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 16, 'label' =&gt; 'Autoimmune', 'sort_id' =&gt; 16],</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lipids and more labs
</commit_message>
<xml_diff>
--- a/storage/lab_lookup.xlsx
+++ b/storage/lab_lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stringali/www/cprs-labs/storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB5B9FB-88C2-FB43-B8B8-A9E729D34B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D4DA5D-001A-794D-B31E-30CC35164333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" xr2:uid="{EC4C72D0-1B9F-7D49-8CE6-24171288DA42}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="311">
   <si>
     <t>WBC</t>
   </si>
@@ -904,6 +904,72 @@
   </si>
   <si>
     <t>CREATININE,Urine</t>
+  </si>
+  <si>
+    <t>IPF</t>
+  </si>
+  <si>
+    <t>COVID-19 (BIOFIRE)</t>
+  </si>
+  <si>
+    <t>HEMOGLOBIN A1C,blood</t>
+  </si>
+  <si>
+    <t>Hbg A1C</t>
+  </si>
+  <si>
+    <t>VITAMIN D 25-OH *TOTAL,Blood</t>
+  </si>
+  <si>
+    <t>Vit D 25-OH</t>
+  </si>
+  <si>
+    <t>Lipids</t>
+  </si>
+  <si>
+    <t>CHOLESTEROL,Blood</t>
+  </si>
+  <si>
+    <t>TRIGLYCERIDE,Blood</t>
+  </si>
+  <si>
+    <t>HDL,blood</t>
+  </si>
+  <si>
+    <t>LDL CALCULATION,blood</t>
+  </si>
+  <si>
+    <t>HDL</t>
+  </si>
+  <si>
+    <t>LDL (calc)</t>
+  </si>
+  <si>
+    <t>Total Cholesterol</t>
+  </si>
+  <si>
+    <t>Triglyceride</t>
+  </si>
+  <si>
+    <t>EGFR,blood</t>
+  </si>
+  <si>
+    <t>EAG</t>
+  </si>
+  <si>
+    <t>Est Avg Glucose</t>
+  </si>
+  <si>
+    <t>MICROALBUMIN,Urine</t>
+  </si>
+  <si>
+    <t>MALB/CREAT RATIO,urine</t>
+  </si>
+  <si>
+    <t>MAU</t>
+  </si>
+  <si>
+    <t>MAU/CR</t>
   </si>
 </sst>
 </file>
@@ -1255,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD366CC-41DC-0B48-90D3-657EFDB6DEEB}">
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="E144" sqref="E2:E144"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1315,7 +1381,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E68" si="0">"['panel_id' =&gt; '"&amp;A3&amp;"', 'name' =&gt; '"&amp;B3&amp;"', 'label' =&gt; '"&amp;C3&amp;"', 'sort_id' =&gt; '"&amp;D3&amp;"'],"</f>
+        <f t="shared" ref="E3:E70" si="0">"['panel_id' =&gt; '"&amp;A3&amp;"', 'name' =&gt; '"&amp;B3&amp;"', 'label' =&gt; '"&amp;C3&amp;"', 'sort_id' =&gt; '"&amp;D3&amp;"'],"</f>
         <v>['panel_id' =&gt; '1', 'name' =&gt; 'RBC', 'label' =&gt; 'RBC', 'sort_id' =&gt; '2'],</v>
       </c>
     </row>
@@ -1432,17 +1498,17 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>289</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>289</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'RDW-CV', 'label' =&gt; 'RDW-CV', 'sort_id' =&gt; '9'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'IPF', 'label' =&gt; 'IPF', 'sort_id' =&gt; '9'],</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1450,17 +1516,17 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NRBC%', 'label' =&gt; 'NRBC%', 'sort_id' =&gt; '10'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'RDW-CV', 'label' =&gt; 'RDW-CV', 'sort_id' =&gt; '9'],</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1468,17 +1534,17 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>11</v>
-      </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NRBC#', 'label' =&gt; 'NRBC#', 'sort_id' =&gt; '11'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NRBC%', 'label' =&gt; 'NRBC%', 'sort_id' =&gt; '10'],</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1486,17 +1552,17 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NEUTROPHILS %', 'label' =&gt; 'Neutrophils %', 'sort_id' =&gt; '12'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NRBC#', 'label' =&gt; 'NRBC#', 'sort_id' =&gt; '11'],</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1504,17 +1570,17 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14">
-        <v>13</v>
-      </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'LYMPHOCYTES %', 'label' =&gt; 'Lymphocytes %', 'sort_id' =&gt; '13'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NEUTROPHILS %', 'label' =&gt; 'Neutrophils %', 'sort_id' =&gt; '12'],</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1522,17 +1588,17 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15">
-        <v>14</v>
-      </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MONOCYTES %', 'label' =&gt; 'Monocytes %', 'sort_id' =&gt; '14'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'LYMPHOCYTES %', 'label' =&gt; 'Lymphocytes %', 'sort_id' =&gt; '13'],</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1540,17 +1606,17 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16">
-        <v>15</v>
-      </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'EOSINOPHILS %', 'label' =&gt; 'Eosinophils %', 'sort_id' =&gt; '15'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MONOCYTES %', 'label' =&gt; 'Monocytes %', 'sort_id' =&gt; '14'],</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1558,17 +1624,17 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17">
-        <v>16</v>
-      </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'BASOPHILS %', 'label' =&gt; 'Basophils %', 'sort_id' =&gt; '16'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'EOSINOPHILS %', 'label' =&gt; 'Eosinophils %', 'sort_id' =&gt; '15'],</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1576,17 +1642,17 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18">
-        <v>17</v>
-      </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'IMMATURE GRANULOCYTE %', 'label' =&gt; 'Immature Granulocyte %', 'sort_id' =&gt; '17'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'BASOPHILS %', 'label' =&gt; 'Basophils %', 'sort_id' =&gt; '16'],</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1594,17 +1660,17 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19">
-        <v>18</v>
-      </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NEUTROPHILS #', 'label' =&gt; 'Neutrophils #', 'sort_id' =&gt; '18'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'IMMATURE GRANULOCYTE %', 'label' =&gt; 'Immature Granulocyte %', 'sort_id' =&gt; '17'],</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1612,17 +1678,17 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
-        <v>19</v>
-      </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'LYMPHOCYTES #', 'label' =&gt; 'Lymphocytes #', 'sort_id' =&gt; '19'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NEUTROPHILS #', 'label' =&gt; 'Neutrophils #', 'sort_id' =&gt; '18'],</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1630,17 +1696,17 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>19</v>
       </c>
-      <c r="C21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21">
-        <v>20</v>
-      </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MONOCYTES #', 'label' =&gt; 'Eosinophils #', 'sort_id' =&gt; '20'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'LYMPHOCYTES #', 'label' =&gt; 'Lymphocytes #', 'sort_id' =&gt; '19'],</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1648,17 +1714,17 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22">
         <v>20</v>
       </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22">
-        <v>21</v>
-      </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'EOSINOPHILS #', 'label' =&gt; 'EOSINOPHILS #', 'sort_id' =&gt; '21'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MONOCYTES #', 'label' =&gt; 'Eosinophils #', 'sort_id' =&gt; '20'],</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1666,17 +1732,17 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23">
         <v>21</v>
       </c>
-      <c r="C23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D23">
-        <v>22</v>
-      </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'BASOPHILS #', 'label' =&gt; 'Basophils #', 'sort_id' =&gt; '22'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'EOSINOPHILS #', 'label' =&gt; 'EOSINOPHILS #', 'sort_id' =&gt; '21'],</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1684,17 +1750,17 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24">
-        <v>23</v>
-      </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'IMMATURE GRANULOCYTE #', 'label' =&gt; 'Immature Granulocyte #', 'sort_id' =&gt; '23'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'BASOPHILS #', 'label' =&gt; 'Basophils #', 'sort_id' =&gt; '22'],</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1702,17 +1768,17 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
-        <v>124</v>
-      </c>
-      <c r="D25">
-        <v>24</v>
-      </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NEUTROPHILS %(M)', 'label' =&gt; 'Neutrophils %(M)', 'sort_id' =&gt; '24'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'IMMATURE GRANULOCYTE #', 'label' =&gt; 'Immature Granulocyte #', 'sort_id' =&gt; '23'],</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1720,17 +1786,17 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
-        <v>125</v>
-      </c>
-      <c r="D26">
-        <v>25</v>
-      </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'LYMPHOCYTES %(M)', 'label' =&gt; 'Lymphocytes %(M)', 'sort_id' =&gt; '25'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NEUTROPHILS %(M)', 'label' =&gt; 'Neutrophils %(M)', 'sort_id' =&gt; '24'],</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1738,17 +1804,17 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
-        <v>126</v>
-      </c>
-      <c r="D27">
-        <v>26</v>
-      </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MONOCYTES %(M)', 'label' =&gt; 'Monocytes %(M)', 'sort_id' =&gt; '26'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'LYMPHOCYTES %(M)', 'label' =&gt; 'Lymphocytes %(M)', 'sort_id' =&gt; '25'],</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1756,17 +1822,17 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28">
-        <v>27</v>
-      </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'EOSINOPHILS %(M)', 'label' =&gt; 'Eosinophils %(M)', 'sort_id' =&gt; '27'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MONOCYTES %(M)', 'label' =&gt; 'Monocytes %(M)', 'sort_id' =&gt; '26'],</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1774,17 +1840,17 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29">
-        <v>28</v>
-      </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'BASOPHILS %(M)', 'label' =&gt; 'Basophils %(M)', 'sort_id' =&gt; '28'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'EOSINOPHILS %(M)', 'label' =&gt; 'Eosinophils %(M)', 'sort_id' =&gt; '27'],</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1792,17 +1858,17 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30">
-        <v>29</v>
-      </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MYELOCYTE %(M)', 'label' =&gt; 'Myelocyte %(M)', 'sort_id' =&gt; '29'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'BASOPHILS %(M)', 'label' =&gt; 'Basophils %(M)', 'sort_id' =&gt; '28'],</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1810,17 +1876,17 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31">
         <v>29</v>
       </c>
-      <c r="C31" t="s">
-        <v>130</v>
-      </c>
-      <c r="D31">
-        <v>30</v>
-      </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'METAMYELOCYTE %(M)', 'label' =&gt; 'Metamyelocyte %(M)', 'sort_id' =&gt; '30'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MYELOCYTE %(M)', 'label' =&gt; 'Myelocyte %(M)', 'sort_id' =&gt; '29'],</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1828,17 +1894,17 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32">
         <v>30</v>
       </c>
-      <c r="C32" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32">
-        <v>31</v>
-      </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NEUTROPHILS #(M)', 'label' =&gt; 'Neutrophils #(M)', 'sort_id' =&gt; '31'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'METAMYELOCYTE %(M)', 'label' =&gt; 'Metamyelocyte %(M)', 'sort_id' =&gt; '30'],</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1846,17 +1912,17 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33">
         <v>31</v>
       </c>
-      <c r="C33" t="s">
-        <v>132</v>
-      </c>
-      <c r="D33">
-        <v>32</v>
-      </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'LYMPHOCYTES #(M)', 'label' =&gt; 'Lymphocytes #(M)', 'sort_id' =&gt; '32'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'NEUTROPHILS #(M)', 'label' =&gt; 'Neutrophils #(M)', 'sort_id' =&gt; '31'],</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1864,17 +1930,17 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34">
         <v>32</v>
       </c>
-      <c r="C34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D34">
-        <v>33</v>
-      </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MONOCYTES #(M)', 'label' =&gt; 'Monocytes #(M)', 'sort_id' =&gt; '33'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'LYMPHOCYTES #(M)', 'label' =&gt; 'Lymphocytes #(M)', 'sort_id' =&gt; '32'],</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1882,17 +1948,17 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35">
         <v>33</v>
       </c>
-      <c r="C35" t="s">
-        <v>134</v>
-      </c>
-      <c r="D35">
-        <v>34</v>
-      </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'EOSINOPHILS #(M)', 'label' =&gt; 'Eosinophils #(M)', 'sort_id' =&gt; '34'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'MONOCYTES #(M)', 'label' =&gt; 'Monocytes #(M)', 'sort_id' =&gt; '33'],</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1900,17 +1966,17 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36">
         <v>34</v>
       </c>
-      <c r="C36" t="s">
-        <v>135</v>
-      </c>
-      <c r="D36">
-        <v>35</v>
-      </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'BASOPHILS #(M)', 'label' =&gt; 'Basophils #(M)', 'sort_id' =&gt; '35'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'EOSINOPHILS #(M)', 'label' =&gt; 'Eosinophils #(M)', 'sort_id' =&gt; '34'],</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1918,35 +1984,35 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37">
         <v>35</v>
       </c>
-      <c r="C37" t="s">
-        <v>136</v>
-      </c>
-      <c r="D37">
-        <v>36</v>
-      </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '1', 'name' =&gt; 'IMMATURE GRANULOCYTE #(M)', 'label' =&gt; 'Immature Granulocyte #(M)', 'sort_id' =&gt; '36'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'BASOPHILS #(M)', 'label' =&gt; 'Basophils #(M)', 'sort_id' =&gt; '35'],</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38">
         <v>36</v>
       </c>
-      <c r="C38" t="s">
-        <v>137</v>
-      </c>
-      <c r="D38">
-        <v>37</v>
-      </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'RBC MORPHOLOGY', 'label' =&gt; 'RBC Morphology', 'sort_id' =&gt; '37'],</v>
+        <v>['panel_id' =&gt; '1', 'name' =&gt; 'IMMATURE GRANULOCYTE #(M)', 'label' =&gt; 'Immature Granulocyte #(M)', 'sort_id' =&gt; '36'],</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1954,17 +2020,17 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39">
         <v>37</v>
       </c>
-      <c r="C39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39">
-        <v>38</v>
-      </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'PLT (ESTM)', 'label' =&gt; 'PLT (ESTM)', 'sort_id' =&gt; '38'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'RBC MORPHOLOGY', 'label' =&gt; 'RBC Morphology', 'sort_id' =&gt; '37'],</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1972,17 +2038,17 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40">
         <v>38</v>
       </c>
-      <c r="C40" t="s">
-        <v>138</v>
-      </c>
-      <c r="D40">
-        <v>39</v>
-      </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'PLT MORPHOLOGY', 'label' =&gt; 'PLT Morphology', 'sort_id' =&gt; '39'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'PLT (ESTM)', 'label' =&gt; 'PLT (ESTM)', 'sort_id' =&gt; '38'],</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1990,17 +2056,17 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41">
         <v>39</v>
       </c>
-      <c r="C41" t="s">
-        <v>139</v>
-      </c>
-      <c r="D41">
-        <v>40</v>
-      </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'LARGE PLATELETS', 'label' =&gt; 'Large Platelets', 'sort_id' =&gt; '40'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'PLT MORPHOLOGY', 'label' =&gt; 'PLT Morphology', 'sort_id' =&gt; '39'],</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2008,17 +2074,17 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42">
         <v>40</v>
       </c>
-      <c r="C42" t="s">
-        <v>140</v>
-      </c>
-      <c r="D42">
-        <v>41</v>
-      </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'POLYCHROMASIA', 'label' =&gt; 'Polychromasia', 'sort_id' =&gt; '41'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'LARGE PLATELETS', 'label' =&gt; 'Large Platelets', 'sort_id' =&gt; '40'],</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2026,17 +2092,17 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43">
         <v>41</v>
       </c>
-      <c r="C43" t="s">
-        <v>141</v>
-      </c>
-      <c r="D43">
-        <v>42</v>
-      </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'HYPOCHROMIA', 'label' =&gt; 'Hypochromia', 'sort_id' =&gt; '42'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'POLYCHROMASIA', 'label' =&gt; 'Polychromasia', 'sort_id' =&gt; '41'],</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2044,17 +2110,17 @@
         <v>2</v>
       </c>
       <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44">
         <v>42</v>
       </c>
-      <c r="C44" t="s">
-        <v>142</v>
-      </c>
-      <c r="D44">
-        <v>43</v>
-      </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'ANISOCYTOSIS', 'label' =&gt; 'Anisocytosis', 'sort_id' =&gt; '43'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'HYPOCHROMIA', 'label' =&gt; 'Hypochromia', 'sort_id' =&gt; '42'],</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2062,17 +2128,17 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45">
         <v>43</v>
       </c>
-      <c r="C45" t="s">
-        <v>143</v>
-      </c>
-      <c r="D45">
-        <v>44</v>
-      </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'MICROCYTOSIS', 'label' =&gt; 'Microcytosis', 'sort_id' =&gt; '44'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'ANISOCYTOSIS', 'label' =&gt; 'Anisocytosis', 'sort_id' =&gt; '43'],</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2080,17 +2146,17 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46">
         <v>44</v>
       </c>
-      <c r="C46" t="s">
-        <v>144</v>
-      </c>
-      <c r="D46">
-        <v>45</v>
-      </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'MACROCYTOSIS', 'label' =&gt; 'Macrocytosis', 'sort_id' =&gt; '45'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'MICROCYTOSIS', 'label' =&gt; 'Microcytosis', 'sort_id' =&gt; '44'],</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2098,17 +2164,17 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" t="s">
+        <v>144</v>
+      </c>
+      <c r="D47">
         <v>45</v>
       </c>
-      <c r="C47" t="s">
-        <v>145</v>
-      </c>
-      <c r="D47">
-        <v>46</v>
-      </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'POIKILOCYTOSIS', 'label' =&gt; 'Poikilocytosis', 'sort_id' =&gt; '46'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'MACROCYTOSIS', 'label' =&gt; 'Macrocytosis', 'sort_id' =&gt; '45'],</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2116,17 +2182,17 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>263</v>
+        <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>264</v>
+        <v>145</v>
       </c>
       <c r="D48">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'TARGET CELLS', 'label' =&gt; 'Target Cells', 'sort_id' =&gt; '47'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'POIKILOCYTOSIS', 'label' =&gt; 'Poikilocytosis', 'sort_id' =&gt; '46'],</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -2134,17 +2200,17 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>263</v>
       </c>
       <c r="C49" t="s">
-        <v>146</v>
+        <v>264</v>
       </c>
       <c r="D49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'SCHISTOCYTES', 'label' =&gt; 'Schistocytes', 'sort_id' =&gt; '48'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'TARGET CELLS', 'label' =&gt; 'Target Cells', 'sort_id' =&gt; '47'],</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -2152,17 +2218,17 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D50">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'SPHEROCYTES', 'label' =&gt; 'Spherocytes', 'sort_id' =&gt; '49'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'SCHISTOCYTES', 'label' =&gt; 'Schistocytes', 'sort_id' =&gt; '48'],</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2170,17 +2236,17 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D51">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'OVALOCYTES', 'label' =&gt; 'Ovalocytes', 'sort_id' =&gt; '50'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'SPHEROCYTES', 'label' =&gt; 'Spherocytes', 'sort_id' =&gt; '49'],</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2188,17 +2254,17 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D52">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'STOMATOCYTE', 'label' =&gt; 'Stomatocyte', 'sort_id' =&gt; '51'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'OVALOCYTES', 'label' =&gt; 'Ovalocytes', 'sort_id' =&gt; '50'],</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2206,17 +2272,17 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D53">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'BURR CELLS', 'label' =&gt; 'Burr cells', 'sort_id' =&gt; '52'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'STOMATOCYTE', 'label' =&gt; 'Stomatocyte', 'sort_id' =&gt; '51'],</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2224,17 +2290,17 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D54">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'ACANTHOCYTES', 'label' =&gt; 'Acanthocytes', 'sort_id' =&gt; '53'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'BURR CELLS', 'label' =&gt; 'Burr cells', 'sort_id' =&gt; '52'],</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2242,35 +2308,35 @@
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D55">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '2', 'name' =&gt; 'TEARDROP CELLS', 'label' =&gt; 'Teardrop cells', 'sort_id' =&gt; '54'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'ACANTHOCYTES', 'label' =&gt; 'Acanthocytes', 'sort_id' =&gt; '53'],</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D56">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'GLUCOSE,Blood', 'label' =&gt; 'Glucose', 'sort_id' =&gt; '55'],</v>
+        <v>['panel_id' =&gt; '2', 'name' =&gt; 'TEARDROP CELLS', 'label' =&gt; 'Teardrop cells', 'sort_id' =&gt; '54'],</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2278,17 +2344,17 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>285</v>
+        <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>284</v>
+        <v>153</v>
       </c>
       <c r="D57">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'GLUCOSE,POC', 'label' =&gt; 'Glucose, POC', 'sort_id' =&gt; '56'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'GLUCOSE,Blood', 'label' =&gt; 'Glucose', 'sort_id' =&gt; '1'],</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2296,17 +2362,17 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>285</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>284</v>
       </c>
       <c r="D58">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'SODIUM,Blood', 'label' =&gt; 'Na', 'sort_id' =&gt; '57'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'GLUCOSE,POC', 'label' =&gt; 'Glucose, POC', 'sort_id' =&gt; '2'],</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2314,17 +2380,17 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D59">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'POTASSIUM,Blood', 'label' =&gt; 'K', 'sort_id' =&gt; '58'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'SODIUM,Blood', 'label' =&gt; 'Na', 'sort_id' =&gt; '3'],</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2332,17 +2398,17 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D60">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CHLORIDE,Blood', 'label' =&gt; 'Cl', 'sort_id' =&gt; '59'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'POTASSIUM,Blood', 'label' =&gt; 'K', 'sort_id' =&gt; '4'],</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2350,17 +2416,17 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>156</v>
       </c>
       <c r="D61">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CARBON DIOXIDE,Blood', 'label' =&gt; 'HCO3', 'sort_id' =&gt; '60'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CHLORIDE,Blood', 'label' =&gt; 'Cl', 'sort_id' =&gt; '5'],</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2368,17 +2434,17 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>78</v>
       </c>
       <c r="D62">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'UREA NITROGEN,Blood', 'label' =&gt; 'BUN', 'sort_id' =&gt; '61'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CARBON DIOXIDE,Blood', 'label' =&gt; 'HCO3', 'sort_id' =&gt; '6'],</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2386,17 +2452,17 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D63">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CREATININE,blood', 'label' =&gt; 'Cr', 'sort_id' =&gt; '62'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'UREA NITROGEN,Blood', 'label' =&gt; 'BUN', 'sort_id' =&gt; '7'],</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2404,17 +2470,17 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D64">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CALCIUM,Blood', 'label' =&gt; 'Calcium', 'sort_id' =&gt; '63'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CREATININE,blood', 'label' =&gt; 'Cr', 'sort_id' =&gt; '8'],</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -2422,17 +2488,17 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D65">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'ANION GAP,blood', 'label' =&gt; 'Anion Gap', 'sort_id' =&gt; '64'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'CALCIUM,Blood', 'label' =&gt; 'Calcium', 'sort_id' =&gt; '9'],</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2440,53 +2506,53 @@
         <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D66">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '3', 'name' =&gt; 'EGFR CKD,blood', 'label' =&gt; 'EGFR', 'sort_id' =&gt; '65'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'ANION GAP,blood', 'label' =&gt; 'Anion Gap', 'sort_id' =&gt; '10'],</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>304</v>
       </c>
       <c r="C67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D67">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="E67" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'PROTEIN,TOTAL,Blood', 'label' =&gt; 'Protein', 'sort_id' =&gt; '66'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'EGFR,blood', 'label' =&gt; 'EGFR', 'sort_id' =&gt; '11'],</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D68">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="0"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALBUMIN ,Blood', 'label' =&gt; 'Albumin', 'sort_id' =&gt; '67'],</v>
+        <v>['panel_id' =&gt; '3', 'name' =&gt; 'EGFR CKD,blood', 'label' =&gt; 'EGFR', 'sort_id' =&gt; '12'],</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2494,17 +2560,17 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C69" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D69">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" ref="E69:E135" si="1">"['panel_id' =&gt; '"&amp;A69&amp;"', 'name' =&gt; '"&amp;B69&amp;"', 'label' =&gt; '"&amp;C69&amp;"', 'sort_id' =&gt; '"&amp;D69&amp;"'],"</f>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'BILIRUBIN,TOTAL,Blood', 'label' =&gt; 'T-Bili', 'sort_id' =&gt; '68'],</v>
+        <f t="shared" si="0"/>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'PROTEIN,TOTAL,Blood', 'label' =&gt; 'Protein', 'sort_id' =&gt; '66'],</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -2512,17 +2578,17 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C70" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D70">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'BILIRUBIN,DIRECT,blood', 'label' =&gt; 'D-Bili', 'sort_id' =&gt; '69'],</v>
+        <f t="shared" si="0"/>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALBUMIN ,Blood', 'label' =&gt; 'Albumin', 'sort_id' =&gt; '67'],</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -2530,17 +2596,17 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C71" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D71">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALKP,Blood', 'label' =&gt; 'ALKP', 'sort_id' =&gt; '70'],</v>
+        <f t="shared" ref="E71:E141" si="1">"['panel_id' =&gt; '"&amp;A71&amp;"', 'name' =&gt; '"&amp;B71&amp;"', 'label' =&gt; '"&amp;C71&amp;"', 'sort_id' =&gt; '"&amp;D71&amp;"'],"</f>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'BILIRUBIN,TOTAL,Blood', 'label' =&gt; 'T-Bili', 'sort_id' =&gt; '68'],</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -2548,17 +2614,17 @@
         <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C72" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D72">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALT,Blood', 'label' =&gt; 'ALT', 'sort_id' =&gt; '71'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'BILIRUBIN,DIRECT,blood', 'label' =&gt; 'D-Bili', 'sort_id' =&gt; '69'],</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -2566,17 +2632,17 @@
         <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C73" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D73">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'AST,Blood', 'label' =&gt; 'AST', 'sort_id' =&gt; '72'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALKP,Blood', 'label' =&gt; 'ALKP', 'sort_id' =&gt; '70'],</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2584,17 +2650,17 @@
         <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D74">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'MAGNESIUM,Blood', 'label' =&gt; 'Mg', 'sort_id' =&gt; '73'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'ALT,Blood', 'label' =&gt; 'ALT', 'sort_id' =&gt; '71'],</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -2602,53 +2668,53 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D75">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '4', 'name' =&gt; 'PHOSPHORUS,Blood', 'label' =&gt; 'PO4', 'sort_id' =&gt; '74'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'AST,Blood', 'label' =&gt; 'AST', 'sort_id' =&gt; '72'],</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B76" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C76" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="D76">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'SODIUM,ISTAT', 'label' =&gt; 'Na', 'sort_id' =&gt; '75'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'MAGNESIUM,Blood', 'label' =&gt; 'Mg', 'sort_id' =&gt; '73'],</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C77" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="D77">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'POTASSIUM,ISTAT', 'label' =&gt; 'K', 'sort_id' =&gt; '76'],</v>
+        <v>['panel_id' =&gt; '4', 'name' =&gt; 'PHOSPHORUS,Blood', 'label' =&gt; 'PO4', 'sort_id' =&gt; '74'],</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2656,17 +2722,17 @@
         <v>5</v>
       </c>
       <c r="B78" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C78" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="D78">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PH @ 37C', 'label' =&gt; 'pH', 'sort_id' =&gt; '77'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'SODIUM,ISTAT', 'label' =&gt; 'Na', 'sort_id' =&gt; '75'],</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2674,17 +2740,17 @@
         <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C79" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="D79">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PCO2 @ 37C', 'label' =&gt; 'PCO2', 'sort_id' =&gt; '78'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'POTASSIUM,ISTAT', 'label' =&gt; 'K', 'sort_id' =&gt; '76'],</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2692,17 +2758,17 @@
         <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C80" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="D80">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E80" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'TCO2', 'label' =&gt; 'TCO2', 'sort_id' =&gt; '79'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PH @ 37C', 'label' =&gt; 'pH', 'sort_id' =&gt; '77'],</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2710,17 +2776,17 @@
         <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C81" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D81">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E81" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PO2 @ 37C', 'label' =&gt; 'PO2', 'sort_id' =&gt; '80'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PCO2 @ 37C', 'label' =&gt; 'PCO2', 'sort_id' =&gt; '78'],</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2728,17 +2794,17 @@
         <v>5</v>
       </c>
       <c r="B82" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C82" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D82">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'HCO3', 'label' =&gt; 'HCO3', 'sort_id' =&gt; '81'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'TCO2', 'label' =&gt; 'TCO2', 'sort_id' =&gt; '79'],</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2746,17 +2812,17 @@
         <v>5</v>
       </c>
       <c r="B83" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D83">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E83" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'BASE EXCESS (BE)', 'label' =&gt; 'Base Excess', 'sort_id' =&gt; '82'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PO2 @ 37C', 'label' =&gt; 'PO2', 'sort_id' =&gt; '80'],</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2764,17 +2830,17 @@
         <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C84" t="s">
-        <v>175</v>
+        <v>78</v>
       </c>
       <c r="D84">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E84" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'O2 SAT%', 'label' =&gt; 'SpO2', 'sort_id' =&gt; '83'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'HCO3', 'label' =&gt; 'HCO3', 'sort_id' =&gt; '81'],</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2782,53 +2848,53 @@
         <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C85" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="D85">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'FIO2', 'label' =&gt; 'FIO2', 'sort_id' =&gt; '84'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'BASE EXCESS (BE)', 'label' =&gt; 'Base Excess', 'sort_id' =&gt; '82'],</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C86" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D86">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '6', 'name' =&gt; 'ANTI-Xa(UFH),BLOOD', 'label' =&gt; 'Anit-Xa (UFH)', 'sort_id' =&gt; '85'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'O2 SAT%', 'label' =&gt; 'SpO2', 'sort_id' =&gt; '83'],</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C87" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
       <c r="D87">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '6', 'name' =&gt; 'PROTHROMBIN TIME,blood', 'label' =&gt; 'PT', 'sort_id' =&gt; '86'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'FIO2', 'label' =&gt; 'FIO2', 'sort_id' =&gt; '84'],</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2836,17 +2902,17 @@
         <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C88" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D88">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '6', 'name' =&gt; 'INR,blood', 'label' =&gt; 'INR', 'sort_id' =&gt; '87'],</v>
+        <v>['panel_id' =&gt; '6', 'name' =&gt; 'ANTI-Xa(UFH),BLOOD', 'label' =&gt; 'Anit-Xa (UFH)', 'sort_id' =&gt; '85'],</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2854,53 +2920,53 @@
         <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C89" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D89">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '6', 'name' =&gt; 'APTT', 'label' =&gt; 'aPTT', 'sort_id' =&gt; '88'],</v>
+        <v>['panel_id' =&gt; '6', 'name' =&gt; 'PROTHROMBIN TIME,blood', 'label' =&gt; 'PT', 'sort_id' =&gt; '86'],</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C90" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D90">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'BNP,BLOOD', 'label' =&gt; 'BNP', 'sort_id' =&gt; '89'],</v>
+        <v>['panel_id' =&gt; '6', 'name' =&gt; 'INR,blood', 'label' =&gt; 'INR', 'sort_id' =&gt; '87'],</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D91">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CK,Blood', 'label' =&gt; 'CK', 'sort_id' =&gt; '90'],</v>
+        <v>['panel_id' =&gt; '6', 'name' =&gt; 'APTT', 'label' =&gt; 'aPTT', 'sort_id' =&gt; '88'],</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2908,17 +2974,17 @@
         <v>7</v>
       </c>
       <c r="B92" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C92" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D92">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CKMB,blood', 'label' =&gt; 'CKMB', 'sort_id' =&gt; '91'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'BNP,BLOOD', 'label' =&gt; 'BNP', 'sort_id' =&gt; '89'],</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2926,17 +2992,17 @@
         <v>7</v>
       </c>
       <c r="B93" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C93" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D93">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CKMB INDEX,blood', 'label' =&gt; 'CKMB Index', 'sort_id' =&gt; '92'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CK,Blood', 'label' =&gt; 'CK', 'sort_id' =&gt; '90'],</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2944,17 +3010,17 @@
         <v>7</v>
       </c>
       <c r="B94" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D94">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'MYOGLOBIN,Blood', 'label' =&gt; 'Myoglobin', 'sort_id' =&gt; '93'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CKMB,blood', 'label' =&gt; 'CKMB', 'sort_id' =&gt; '91'],</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2962,53 +3028,53 @@
         <v>7</v>
       </c>
       <c r="B95" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C95" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D95">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '7', 'name' =&gt; 'TROPONIN-I,BLOOD', 'label' =&gt; 'Troponin-I', 'sort_id' =&gt; '94'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'CKMB INDEX,blood', 'label' =&gt; 'CKMB Index', 'sort_id' =&gt; '92'],</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B96" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C96" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D96">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE GLUCOSE', 'label' =&gt; 'Urine Glucose', 'sort_id' =&gt; '95'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'MYOGLOBIN,Blood', 'label' =&gt; 'Myoglobin', 'sort_id' =&gt; '93'],</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B97" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C97" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D97">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE PROTEIN', 'label' =&gt; 'Urine Protein', 'sort_id' =&gt; '96'],</v>
+        <v>['panel_id' =&gt; '7', 'name' =&gt; 'TROPONIN-I,BLOOD', 'label' =&gt; 'Troponin-I', 'sort_id' =&gt; '94'],</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -3016,17 +3082,17 @@
         <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C98" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D98">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BILIRUBIN', 'label' =&gt; 'Urine Bilirubin', 'sort_id' =&gt; '97'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE GLUCOSE', 'label' =&gt; 'Urine Glucose', 'sort_id' =&gt; '95'],</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -3034,17 +3100,17 @@
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C99" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D99">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE UROBILINOGEN', 'label' =&gt; 'Urine Urobilinogen', 'sort_id' =&gt; '98'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE PROTEIN', 'label' =&gt; 'Urine Protein', 'sort_id' =&gt; '96'],</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -3052,17 +3118,17 @@
         <v>8</v>
       </c>
       <c r="B100" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C100" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D100">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE PH', 'label' =&gt; 'Urine pH', 'sort_id' =&gt; '99'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BILIRUBIN', 'label' =&gt; 'Urine Bilirubin', 'sort_id' =&gt; '97'],</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -3070,17 +3136,17 @@
         <v>8</v>
       </c>
       <c r="B101" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C101" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D101">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BLOOD', 'label' =&gt; 'Urine Blood', 'sort_id' =&gt; '100'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE UROBILINOGEN', 'label' =&gt; 'Urine Urobilinogen', 'sort_id' =&gt; '98'],</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -3088,17 +3154,17 @@
         <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C102" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D102">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE KETONES', 'label' =&gt; 'Urine Ketones', 'sort_id' =&gt; '101'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE PH', 'label' =&gt; 'Urine pH', 'sort_id' =&gt; '99'],</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -3106,17 +3172,17 @@
         <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C103" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D103">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE NITRITE', 'label' =&gt; 'Urine Nitrite', 'sort_id' =&gt; '102'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BLOOD', 'label' =&gt; 'Urine Blood', 'sort_id' =&gt; '100'],</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -3124,17 +3190,17 @@
         <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C104" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D104">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE LEUKOCYTE ESTERASE', 'label' =&gt; 'Urine Leukocyte Esterase', 'sort_id' =&gt; '103'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE KETONES', 'label' =&gt; 'Urine Ketones', 'sort_id' =&gt; '101'],</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -3142,17 +3208,17 @@
         <v>8</v>
       </c>
       <c r="B105" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C105" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D105">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE CLARITY', 'label' =&gt; 'Urine Clarity', 'sort_id' =&gt; '104'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE NITRITE', 'label' =&gt; 'Urine Nitrite', 'sort_id' =&gt; '102'],</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -3160,17 +3226,17 @@
         <v>8</v>
       </c>
       <c r="B106" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C106" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D106">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE SPECIFIC GRAVITY', 'label' =&gt; 'Urine Sp Gravity', 'sort_id' =&gt; '105'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE LEUKOCYTE ESTERASE', 'label' =&gt; 'Urine Leukocyte Esterase', 'sort_id' =&gt; '103'],</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -3178,17 +3244,17 @@
         <v>8</v>
       </c>
       <c r="B107" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C107" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D107">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE COLOR', 'label' =&gt; 'Urine Color', 'sort_id' =&gt; '106'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE CLARITY', 'label' =&gt; 'Urine Clarity', 'sort_id' =&gt; '104'],</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -3196,17 +3262,17 @@
         <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C108" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D108">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'RBC/HPF', 'label' =&gt; 'RBC/Hpf', 'sort_id' =&gt; '107'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE SPECIFIC GRAVITY', 'label' =&gt; 'Urine Sp Gravity', 'sort_id' =&gt; '105'],</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -3214,17 +3280,17 @@
         <v>8</v>
       </c>
       <c r="B109" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C109" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D109">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'WBC/HPF', 'label' =&gt; 'WBC/Hpf', 'sort_id' =&gt; '108'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE COLOR', 'label' =&gt; 'Urine Color', 'sort_id' =&gt; '106'],</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -3232,17 +3298,17 @@
         <v>8</v>
       </c>
       <c r="B110" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C110" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D110">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BACTERIA', 'label' =&gt; 'Urine Bacteria', 'sort_id' =&gt; '109'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'RBC/HPF', 'label' =&gt; 'RBC/Hpf', 'sort_id' =&gt; '107'],</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -3250,17 +3316,17 @@
         <v>8</v>
       </c>
       <c r="B111" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C111" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D111">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'SQUAMOUS EPITHELIAL', 'label' =&gt; 'Squamous Epithelial', 'sort_id' =&gt; '110'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'WBC/HPF', 'label' =&gt; 'WBC/Hpf', 'sort_id' =&gt; '108'],</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -3268,17 +3334,17 @@
         <v>8</v>
       </c>
       <c r="B112" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C112" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D112">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'HYALINE CAST', 'label' =&gt; 'Hyaline Cast', 'sort_id' =&gt; '111'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'URINE BACTERIA', 'label' =&gt; 'Urine Bacteria', 'sort_id' =&gt; '109'],</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -3286,89 +3352,89 @@
         <v>8</v>
       </c>
       <c r="B113" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C113" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D113">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E113" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '8', 'name' =&gt; 'CALCIUM OXALATE', 'label' =&gt; 'Calcium Oxalate', 'sort_id' =&gt; '112'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'SQUAMOUS EPITHELIAL', 'label' =&gt; 'Squamous Epithelial', 'sort_id' =&gt; '110'],</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B114" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C114" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D114">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E114" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '9', 'name' =&gt; 'C. DIFF TOX B GENE PCR,stool', 'label' =&gt; 'C. Diff Tox B PCR', 'sort_id' =&gt; '113'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'HYALINE CAST', 'label' =&gt; 'Hyaline Cast', 'sort_id' =&gt; '111'],</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B115" t="s">
-        <v>208</v>
+        <v>109</v>
       </c>
       <c r="C115" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D115">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E115" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '9', 'name' =&gt; 'VZ DNA', 'label' =&gt; 'VZV DNA PCR', 'sort_id' =&gt; '114'],</v>
+        <v>['panel_id' =&gt; '8', 'name' =&gt; 'CALCIUM OXALATE', 'label' =&gt; 'Calcium Oxalate', 'sort_id' =&gt; '112'],</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B116" t="s">
-        <v>252</v>
+        <v>210</v>
       </c>
       <c r="C116" t="s">
-        <v>253</v>
+        <v>211</v>
       </c>
       <c r="D116">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E116" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'ETHANOL,Urine', 'label' =&gt; 'EtOH', 'sort_id' =&gt; '115'],</v>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'C. DIFF TOX B GENE PCR,stool', 'label' =&gt; 'C. Diff Tox B PCR', 'sort_id' =&gt; '113'],</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="C117" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="D117">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'AMPHETAMINES SCREEN,urine', 'label' =&gt; 'Amphetamines', 'sort_id' =&gt; '116'],</v>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'VZ DNA', 'label' =&gt; 'VZV DNA PCR', 'sort_id' =&gt; '114'],</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -3376,17 +3442,17 @@
         <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="C118" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="D118">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'BARBITURATES SCREEN,urine', 'label' =&gt; 'Barbiturates', 'sort_id' =&gt; '117'],</v>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'ETHANOL,Urine', 'label' =&gt; 'EtOH', 'sort_id' =&gt; '115'],</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -3394,17 +3460,17 @@
         <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C119" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D119">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'BENZODIAZEPINES SCREEN,urine', 'label' =&gt; 'Benzodiazepines', 'sort_id' =&gt; '118'],</v>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'AMPHETAMINES SCREEN,urine', 'label' =&gt; 'Amphetamines', 'sort_id' =&gt; '116'],</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -3412,17 +3478,17 @@
         <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C120" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D120">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'CANNABINOIDS SCREEN,urine', 'label' =&gt; 'Cannabinoids', 'sort_id' =&gt; '119'],</v>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'BARBITURATES SCREEN,urine', 'label' =&gt; 'Barbiturates', 'sort_id' =&gt; '117'],</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -3430,17 +3496,17 @@
         <v>12</v>
       </c>
       <c r="B121" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C121" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D121">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E121" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'COCAINE SCREEN,urine', 'label' =&gt; 'Cocaine', 'sort_id' =&gt; '120'],</v>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'BENZODIAZEPINES SCREEN,urine', 'label' =&gt; 'Benzodiazepines', 'sort_id' =&gt; '118'],</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -3448,17 +3514,17 @@
         <v>12</v>
       </c>
       <c r="B122" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C122" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D122">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E122" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'METHADONE SCREEN,urine', 'label' =&gt; 'Methadone', 'sort_id' =&gt; '121'],</v>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'CANNABINOIDS SCREEN,urine', 'label' =&gt; 'Cannabinoids', 'sort_id' =&gt; '119'],</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -3466,17 +3532,17 @@
         <v>12</v>
       </c>
       <c r="B123" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C123" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D123">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E123" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'OPIATES SCREEN,urine', 'label' =&gt; 'Opiates', 'sort_id' =&gt; '122'],</v>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'COCAINE SCREEN,urine', 'label' =&gt; 'Cocaine', 'sort_id' =&gt; '120'],</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -3484,17 +3550,17 @@
         <v>12</v>
       </c>
       <c r="B124" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C124" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D124">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E124" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'OXYCODONE SCREEN,urine', 'label' =&gt; 'Oxycodone', 'sort_id' =&gt; '123'],</v>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'METHADONE SCREEN,urine', 'label' =&gt; 'Methadone', 'sort_id' =&gt; '121'],</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -3502,107 +3568,107 @@
         <v>12</v>
       </c>
       <c r="B125" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C125" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D125">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '12', 'name' =&gt; 'PHENCYCLIDINE SCREEN,urine', 'label' =&gt; 'Phencyclidine', 'sort_id' =&gt; '124'],</v>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'OPIATES SCREEN,urine', 'label' =&gt; 'Opiates', 'sort_id' =&gt; '122'],</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B126" t="s">
-        <v>288</v>
+        <v>231</v>
       </c>
       <c r="C126" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D126">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E126" t="str">
         <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '11', 'name' =&gt; 'CREATININE,Urine', 'label' =&gt; 'Creatinine, Urine', 'sort_id' =&gt; '125'],</v>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'OXYCODONE SCREEN,urine', 'label' =&gt; 'Oxycodone', 'sort_id' =&gt; '123'],</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B127" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="C127" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="D127">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E127" t="str">
-        <f>"['panel_id' =&gt; '"&amp;A127&amp;"', 'name' =&gt; '"&amp;B127&amp;"', 'label' =&gt; '"&amp;C127&amp;"', 'sort_id' =&gt; '"&amp;D127&amp;"'],"</f>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'TSH,BLOOD', 'label' =&gt; 'TSH', 'sort_id' =&gt; '126'],</v>
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '12', 'name' =&gt; 'PHENCYCLIDINE SCREEN,urine', 'label' =&gt; 'Phencyclidine', 'sort_id' =&gt; '124'],</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>249</v>
+        <v>288</v>
       </c>
       <c r="C128" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="D128">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="E128" t="str">
-        <f>"['panel_id' =&gt; '"&amp;A128&amp;"', 'name' =&gt; '"&amp;B128&amp;"', 'label' =&gt; '"&amp;C128&amp;"', 'sort_id' =&gt; '"&amp;D128&amp;"'],"</f>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'AMMONIA,BLOOD', 'label' =&gt; 'Ammonia', 'sort_id' =&gt; '127'],</v>
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '11', 'name' =&gt; 'CREATININE,Urine', 'label' =&gt; 'Creatinine, Urine', 'sort_id' =&gt; '1'],</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B129" t="s">
-        <v>248</v>
+        <v>307</v>
       </c>
       <c r="C129" t="s">
-        <v>259</v>
+        <v>309</v>
       </c>
       <c r="D129">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="E129" t="str">
-        <f>"['panel_id' =&gt; '"&amp;A129&amp;"', 'name' =&gt; '"&amp;B129&amp;"', 'label' =&gt; '"&amp;C129&amp;"', 'sort_id' =&gt; '"&amp;D129&amp;"'],"</f>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'LACTIC ACID,BLOOD', 'label' =&gt; 'Lactic Acid', 'sort_id' =&gt; '128'],</v>
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '11', 'name' =&gt; 'MICROALBUMIN,Urine', 'label' =&gt; 'MAU', 'sort_id' =&gt; '2'],</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="C130" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="D130">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="E130" t="str">
-        <f>"['panel_id' =&gt; '"&amp;A130&amp;"', 'name' =&gt; '"&amp;B130&amp;"', 'label' =&gt; '"&amp;C130&amp;"', 'sort_id' =&gt; '"&amp;D130&amp;"'],"</f>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'LIPASE,BLOOD', 'label' =&gt; 'Lipase', 'sort_id' =&gt; '129'],</v>
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '11', 'name' =&gt; 'MALB/CREAT RATIO,urine', 'label' =&gt; 'MAU/CR', 'sort_id' =&gt; '3'],</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -3610,17 +3676,17 @@
         <v>5</v>
       </c>
       <c r="B131" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C131" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D131">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="E131" t="str">
         <f>"['panel_id' =&gt; '"&amp;A131&amp;"', 'name' =&gt; '"&amp;B131&amp;"', 'label' =&gt; '"&amp;C131&amp;"', 'sort_id' =&gt; '"&amp;D131&amp;"'],"</f>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'ESR,BLOOD', 'label' =&gt; 'ESR', 'sort_id' =&gt; '130'],</v>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'TSH,BLOOD', 'label' =&gt; 'TSH', 'sort_id' =&gt; '1'],</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -3628,17 +3694,17 @@
         <v>5</v>
       </c>
       <c r="B132" t="s">
-        <v>243</v>
+        <v>291</v>
       </c>
       <c r="C132" t="s">
-        <v>254</v>
+        <v>292</v>
       </c>
       <c r="D132">
-        <v>131</v>
+        <v>2</v>
       </c>
       <c r="E132" t="str">
-        <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'C-REACTIVE PROTEIN,BLOOD', 'label' =&gt; 'CRP', 'sort_id' =&gt; '131'],</v>
+        <f>"['panel_id' =&gt; '"&amp;A132&amp;"', 'name' =&gt; '"&amp;B132&amp;"', 'label' =&gt; '"&amp;C132&amp;"', 'sort_id' =&gt; '"&amp;D132&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'HEMOGLOBIN A1C,blood', 'label' =&gt; 'Hbg A1C', 'sort_id' =&gt; '2'],</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -3646,17 +3712,17 @@
         <v>5</v>
       </c>
       <c r="B133" t="s">
-        <v>244</v>
+        <v>305</v>
       </c>
       <c r="C133" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="D133">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E133" t="str">
-        <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PROCALCITONIN,BLOOD', 'label' =&gt; 'Procalcitonin', 'sort_id' =&gt; '132'],</v>
+        <f>"['panel_id' =&gt; '"&amp;A133&amp;"', 'name' =&gt; '"&amp;B133&amp;"', 'label' =&gt; '"&amp;C133&amp;"', 'sort_id' =&gt; '"&amp;D133&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'EAG', 'label' =&gt; 'Est Avg Glucose', 'sort_id' =&gt; '3'],</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -3664,17 +3730,17 @@
         <v>5</v>
       </c>
       <c r="B134" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C134" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D134">
-        <v>133</v>
+        <v>4</v>
       </c>
       <c r="E134" t="str">
-        <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'VANCOMYCIN-TROUGH,BLOOD', 'label' =&gt; 'Vanco, Trough', 'sort_id' =&gt; '133'],</v>
+        <f>"['panel_id' =&gt; '"&amp;A134&amp;"', 'name' =&gt; '"&amp;B134&amp;"', 'label' =&gt; '"&amp;C134&amp;"', 'sort_id' =&gt; '"&amp;D134&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'AMMONIA,BLOOD', 'label' =&gt; 'Ammonia', 'sort_id' =&gt; '4'],</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -3682,17 +3748,17 @@
         <v>5</v>
       </c>
       <c r="B135" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C135" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D135">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="E135" t="str">
-        <f t="shared" si="1"/>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'VANCOMYCIN-RANDOM,BLOOD', 'label' =&gt; 'Vanco, Random', 'sort_id' =&gt; '134'],</v>
+        <f>"['panel_id' =&gt; '"&amp;A135&amp;"', 'name' =&gt; '"&amp;B135&amp;"', 'label' =&gt; '"&amp;C135&amp;"', 'sort_id' =&gt; '"&amp;D135&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'LACTIC ACID,BLOOD', 'label' =&gt; 'Lactic Acid', 'sort_id' =&gt; '5'],</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -3700,161 +3766,377 @@
         <v>5</v>
       </c>
       <c r="B136" t="s">
-        <v>250</v>
+        <v>286</v>
       </c>
       <c r="C136" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="D136">
-        <v>135</v>
+        <v>6</v>
       </c>
       <c r="E136" t="str">
-        <f t="shared" ref="E136:E144" si="2">"['panel_id' =&gt; '"&amp;A136&amp;"', 'name' =&gt; '"&amp;B136&amp;"', 'label' =&gt; '"&amp;C136&amp;"', 'sort_id' =&gt; '"&amp;D136&amp;"'],"</f>
-        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PROLACTIN,BLOOD', 'label' =&gt; 'Prolactin', 'sort_id' =&gt; '135'],</v>
+        <f>"['panel_id' =&gt; '"&amp;A136&amp;"', 'name' =&gt; '"&amp;B136&amp;"', 'label' =&gt; '"&amp;C136&amp;"', 'sort_id' =&gt; '"&amp;D136&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'LIPASE,BLOOD', 'label' =&gt; 'Lipase', 'sort_id' =&gt; '6'],</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137">
+        <v>5</v>
+      </c>
+      <c r="B137" t="s">
+        <v>247</v>
+      </c>
+      <c r="C137" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137">
+        <v>7</v>
+      </c>
+      <c r="E137" t="str">
+        <f>"['panel_id' =&gt; '"&amp;A137&amp;"', 'name' =&gt; '"&amp;B137&amp;"', 'label' =&gt; '"&amp;C137&amp;"', 'sort_id' =&gt; '"&amp;D137&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'ESR,BLOOD', 'label' =&gt; 'ESR', 'sort_id' =&gt; '7'],</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>5</v>
+      </c>
+      <c r="B138" t="s">
+        <v>243</v>
+      </c>
+      <c r="C138" t="s">
+        <v>254</v>
+      </c>
+      <c r="D138">
+        <v>8</v>
+      </c>
+      <c r="E138" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'C-REACTIVE PROTEIN,BLOOD', 'label' =&gt; 'CRP', 'sort_id' =&gt; '8'],</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>5</v>
+      </c>
+      <c r="B139" t="s">
+        <v>244</v>
+      </c>
+      <c r="C139" t="s">
+        <v>255</v>
+      </c>
+      <c r="D139">
+        <v>9</v>
+      </c>
+      <c r="E139" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PROCALCITONIN,BLOOD', 'label' =&gt; 'Procalcitonin', 'sort_id' =&gt; '9'],</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>5</v>
+      </c>
+      <c r="B140" t="s">
+        <v>245</v>
+      </c>
+      <c r="C140" t="s">
+        <v>257</v>
+      </c>
+      <c r="D140">
+        <v>10</v>
+      </c>
+      <c r="E140" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'VANCOMYCIN-TROUGH,BLOOD', 'label' =&gt; 'Vanco, Trough', 'sort_id' =&gt; '10'],</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>5</v>
+      </c>
+      <c r="B141" t="s">
+        <v>246</v>
+      </c>
+      <c r="C141" t="s">
+        <v>256</v>
+      </c>
+      <c r="D141">
+        <v>11</v>
+      </c>
+      <c r="E141" t="str">
+        <f t="shared" si="1"/>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'VANCOMYCIN-RANDOM,BLOOD', 'label' =&gt; 'Vanco, Random', 'sort_id' =&gt; '11'],</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>5</v>
+      </c>
+      <c r="B142" t="s">
+        <v>250</v>
+      </c>
+      <c r="C142" t="s">
+        <v>261</v>
+      </c>
+      <c r="D142">
+        <v>12</v>
+      </c>
+      <c r="E142" t="str">
+        <f t="shared" ref="E142:E156" si="2">"['panel_id' =&gt; '"&amp;A142&amp;"', 'name' =&gt; '"&amp;B142&amp;"', 'label' =&gt; '"&amp;C142&amp;"', 'sort_id' =&gt; '"&amp;D142&amp;"'],"</f>
+        <v>['panel_id' =&gt; '5', 'name' =&gt; 'PROLACTIN,BLOOD', 'label' =&gt; 'Prolactin', 'sort_id' =&gt; '12'],</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
         <v>15</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B143" t="s">
         <v>268</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C143" t="s">
         <v>270</v>
       </c>
-      <c r="D137">
+      <c r="D143">
         <v>136</v>
       </c>
-      <c r="E137" t="str">
+      <c r="E143" t="str">
         <f t="shared" si="2"/>
         <v>['panel_id' =&gt; '15', 'name' =&gt; 'FOLATE,Blood', 'label' =&gt; 'Folate', 'sort_id' =&gt; '136'],</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144">
         <v>15</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B144" t="s">
         <v>269</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C144" t="s">
         <v>271</v>
       </c>
-      <c r="D138">
+      <c r="D144">
         <v>137</v>
       </c>
-      <c r="E138" t="str">
+      <c r="E144" t="str">
         <f t="shared" si="2"/>
         <v>['panel_id' =&gt; '15', 'name' =&gt; 'VITAMIN B12,Blood', 'label' =&gt; 'Vit B12', 'sort_id' =&gt; '137'],</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>15</v>
+      </c>
+      <c r="B145" t="s">
+        <v>293</v>
+      </c>
+      <c r="C145" t="s">
+        <v>294</v>
+      </c>
+      <c r="D145">
+        <v>138</v>
+      </c>
+      <c r="E145" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '15', 'name' =&gt; 'VITAMIN D 25-OH *TOTAL,Blood', 'label' =&gt; 'Vit D 25-OH', 'sort_id' =&gt; '138'],</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146">
         <v>9</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B146" t="s">
+        <v>290</v>
+      </c>
+      <c r="C146" t="s">
+        <v>277</v>
+      </c>
+      <c r="D146">
+        <v>137</v>
+      </c>
+      <c r="E146" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '9', 'name' =&gt; 'COVID-19 (BIOFIRE)', 'label' =&gt; 'COVID-19 PCR', 'sort_id' =&gt; '137'],</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>9</v>
+      </c>
+      <c r="B147" t="s">
         <v>272</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C147" t="s">
         <v>277</v>
       </c>
-      <c r="D139">
+      <c r="D147">
         <v>138</v>
       </c>
-      <c r="E139" t="str">
+      <c r="E147" t="str">
         <f t="shared" si="2"/>
         <v>['panel_id' =&gt; '9', 'name' =&gt; 'COVID-19 (CEPHEID)', 'label' =&gt; 'COVID-19 PCR', 'sort_id' =&gt; '138'],</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148">
         <v>9</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B148" t="s">
         <v>273</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C148" t="s">
         <v>276</v>
       </c>
-      <c r="D140">
+      <c r="D148">
         <v>139</v>
       </c>
-      <c r="E140" t="str">
+      <c r="E148" t="str">
         <f t="shared" si="2"/>
         <v>['panel_id' =&gt; '9', 'name' =&gt; 'COVID-19 ANTIGEN (BINAX)', 'label' =&gt; 'COVID-19 Antigen', 'sort_id' =&gt; '139'],</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149">
         <v>9</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B149" t="s">
         <v>274</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C149" t="s">
         <v>277</v>
       </c>
-      <c r="D141">
+      <c r="D149">
         <v>140</v>
       </c>
-      <c r="E141" t="str">
+      <c r="E149" t="str">
         <f t="shared" si="2"/>
         <v>['panel_id' =&gt; '9', 'name' =&gt; 'COVID-19 PCR (FLUVID)', 'label' =&gt; 'COVID-19 PCR', 'sort_id' =&gt; '140'],</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150">
         <v>9</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B150" t="s">
         <v>283</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C150" t="s">
         <v>278</v>
       </c>
-      <c r="D142">
+      <c r="D150">
         <v>141</v>
       </c>
-      <c r="E142" t="str">
+      <c r="E150" t="str">
         <f t="shared" si="2"/>
         <v>['panel_id' =&gt; '9', 'name' =&gt; 'FLU A PCR (FLUVID)', 'label' =&gt; 'FLU A PCR', 'sort_id' =&gt; '141'],</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151">
         <v>9</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B151" t="s">
         <v>275</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C151" t="s">
         <v>279</v>
       </c>
-      <c r="D143">
+      <c r="D151">
         <v>142</v>
       </c>
-      <c r="E143" t="str">
+      <c r="E151" t="str">
         <f t="shared" si="2"/>
         <v>['panel_id' =&gt; '9', 'name' =&gt; 'FLU B PCR (FLUVID)', 'label' =&gt; 'FLU B PCR', 'sort_id' =&gt; '142'],</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152">
         <v>9</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B152" t="s">
         <v>282</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C152" t="s">
         <v>280</v>
       </c>
-      <c r="D144">
+      <c r="D152">
         <v>143</v>
       </c>
-      <c r="E144" t="str">
+      <c r="E152" t="str">
         <f t="shared" si="2"/>
         <v>['panel_id' =&gt; '9', 'name' =&gt; 'RSV PCR (FLUVID)', 'label' =&gt; 'RSV PCR', 'sort_id' =&gt; '143'],</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>17</v>
+      </c>
+      <c r="B153" t="s">
+        <v>296</v>
+      </c>
+      <c r="C153" t="s">
+        <v>302</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="E153" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '17', 'name' =&gt; 'CHOLESTEROL,Blood', 'label' =&gt; 'Total Cholesterol', 'sort_id' =&gt; '1'],</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>17</v>
+      </c>
+      <c r="B154" t="s">
+        <v>297</v>
+      </c>
+      <c r="C154" t="s">
+        <v>303</v>
+      </c>
+      <c r="D154">
+        <v>2</v>
+      </c>
+      <c r="E154" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '17', 'name' =&gt; 'TRIGLYCERIDE,Blood', 'label' =&gt; 'Triglyceride', 'sort_id' =&gt; '2'],</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>17</v>
+      </c>
+      <c r="B155" t="s">
+        <v>298</v>
+      </c>
+      <c r="C155" t="s">
+        <v>300</v>
+      </c>
+      <c r="D155">
+        <v>3</v>
+      </c>
+      <c r="E155" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '17', 'name' =&gt; 'HDL,blood', 'label' =&gt; 'HDL', 'sort_id' =&gt; '3'],</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>17</v>
+      </c>
+      <c r="B156" t="s">
+        <v>299</v>
+      </c>
+      <c r="C156" t="s">
+        <v>301</v>
+      </c>
+      <c r="D156">
+        <v>4</v>
+      </c>
+      <c r="E156" t="str">
+        <f t="shared" si="2"/>
+        <v>['panel_id' =&gt; '17', 'name' =&gt; 'LDL CALCULATION,blood', 'label' =&gt; 'LDL (calc)', 'sort_id' =&gt; '4'],</v>
       </c>
     </row>
   </sheetData>
@@ -3865,10 +4147,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC0B4A5-5A2B-6C43-ADFA-43D0E3B93788}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3913,7 +4195,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D17" si="0">"['id' =&gt; "&amp;A3 &amp;", 'label' =&gt; '"&amp;B3 &amp;"', 'sort_id' =&gt; "&amp;C3 &amp;"],"</f>
+        <f t="shared" ref="D3:D18" si="0">"['id' =&gt; "&amp;A3 &amp;", 'label' =&gt; '"&amp;B3 &amp;"', 'sort_id' =&gt; "&amp;C3 &amp;"],"</f>
         <v>['id' =&gt; 2, 'label' =&gt; 'Morphology', 'sort_id' =&gt; 2],</v>
       </c>
     </row>
@@ -4015,11 +4297,11 @@
         <v>220</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>['id' =&gt; 9, 'label' =&gt; 'Infectious', 'sort_id' =&gt; 10],</v>
+        <v>['id' =&gt; 9, 'label' =&gt; 'Infectious', 'sort_id' =&gt; 11],</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4030,11 +4312,11 @@
         <v>221</v>
       </c>
       <c r="C11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>['id' =&gt; 10, 'label' =&gt; 'Body Fluids', 'sort_id' =&gt; 11],</v>
+        <v>['id' =&gt; 10, 'label' =&gt; 'Body Fluids', 'sort_id' =&gt; 12],</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4045,11 +4327,11 @@
         <v>222</v>
       </c>
       <c r="C12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>['id' =&gt; 11, 'label' =&gt; 'Urine', 'sort_id' =&gt; 12],</v>
+        <v>['id' =&gt; 11, 'label' =&gt; 'Urine', 'sort_id' =&gt; 13],</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4060,11 +4342,11 @@
         <v>223</v>
       </c>
       <c r="C13">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>['id' =&gt; 12, 'label' =&gt; 'UDS', 'sort_id' =&gt; 13],</v>
+        <v>['id' =&gt; 12, 'label' =&gt; 'UDS', 'sort_id' =&gt; 14],</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4090,11 +4372,11 @@
         <v>265</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>['id' =&gt; 14, 'label' =&gt; 'Iron', 'sort_id' =&gt; 14],</v>
+        <v>['id' =&gt; 14, 'label' =&gt; 'Iron', 'sort_id' =&gt; 15],</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4105,11 +4387,11 @@
         <v>266</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>['id' =&gt; 15, 'label' =&gt; 'Vitamins', 'sort_id' =&gt; 15],</v>
+        <v>['id' =&gt; 15, 'label' =&gt; 'Vitamins', 'sort_id' =&gt; 16],</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -4120,11 +4402,26 @@
         <v>267</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>['id' =&gt; 16, 'label' =&gt; 'Autoimmune', 'sort_id' =&gt; 16],</v>
+        <v>['id' =&gt; 16, 'label' =&gt; 'Autoimmune', 'sort_id' =&gt; 17],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>295</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>['id' =&gt; 17, 'label' =&gt; 'Lipids', 'sort_id' =&gt; 10],</v>
       </c>
     </row>
   </sheetData>

</xml_diff>